<commit_message>
CloneWorks pair wise result to Class wise result conversion completed. This will save a lot of memory to be process
</commit_message>
<xml_diff>
--- a/data_files/final_dataset_jss/processed_result.xlsx
+++ b/data_files/final_dataset_jss/processed_result.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdn769\FindCochangeByClone\data_files\final_dataset_jss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA103E5-265A-4786-B19B-54676CA96E63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE24ACD1-65AF-40FE-A9C6-71519B79F9C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-4404" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Recall" sheetId="1" r:id="rId1"/>
+    <sheet name="Result" sheetId="1" r:id="rId1"/>
+    <sheet name="cw_separate_types" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
   <si>
     <t>ccfinder</t>
   </si>
@@ -102,6 +103,18 @@
   </si>
   <si>
     <t>F1 Scores</t>
+  </si>
+  <si>
+    <t>cw_type1</t>
+  </si>
+  <si>
+    <t>cw_type2blind</t>
+  </si>
+  <si>
+    <t>cw_type3pattern</t>
+  </si>
+  <si>
+    <t>cw_type3token</t>
   </si>
 </sst>
 </file>
@@ -145,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -155,15 +168,24 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,28 +490,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="N1" s="4" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="N1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -720,31 +742,31 @@
       <c r="L5" s="2">
         <v>4.6507884151442046E-2</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="5">
         <v>0.34246383000000002</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="5">
         <v>0.16423603000000001</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="5">
         <v>0.24050800999999999</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="5">
         <v>0.16705046000000001</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R5" s="5">
         <v>6.1724910000000001E-2</v>
       </c>
-      <c r="S5" s="6">
+      <c r="S5" s="5">
         <v>0.17220925000000001</v>
       </c>
-      <c r="T5" s="6">
+      <c r="T5" s="5">
         <v>0.25656886000000001</v>
       </c>
-      <c r="U5" s="6">
+      <c r="U5" s="5">
         <v>0.26182491000000002</v>
       </c>
-      <c r="V5" s="6">
+      <c r="V5" s="5">
         <v>0.16842712000000001</v>
       </c>
     </row>
@@ -785,31 +807,31 @@
       <c r="L6" s="2">
         <v>0.10301625457875457</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="5">
         <v>0.19669489000000001</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="5">
         <v>9.5825530000000006E-2</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="5">
         <v>0.1803826</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="5">
         <v>0.12524266000000001</v>
       </c>
-      <c r="R6" s="6">
+      <c r="R6" s="5">
         <v>4.1971370000000001E-2</v>
       </c>
-      <c r="S6" s="6">
+      <c r="S6" s="5">
         <v>0.10716726</v>
       </c>
-      <c r="T6" s="6">
+      <c r="T6" s="5">
         <v>0.18308652</v>
       </c>
-      <c r="U6" s="6">
+      <c r="U6" s="5">
         <v>4.329028E-2</v>
       </c>
-      <c r="V6" s="6">
+      <c r="V6" s="5">
         <v>0.13776347999999999</v>
       </c>
     </row>
@@ -873,31 +895,31 @@
       <c r="L8" s="2">
         <v>4.8361742287394344E-2</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="5">
         <v>0.21877938999999999</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="5">
         <v>0.10597388000000001</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="5">
         <v>0.19811214999999999</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="5">
         <v>9.0702859999999996E-2</v>
       </c>
-      <c r="R8" s="6">
+      <c r="R8" s="5">
         <v>4.2192130000000001E-2</v>
       </c>
-      <c r="S8" s="6">
+      <c r="S8" s="5">
         <v>0.1597181</v>
       </c>
-      <c r="T8" s="6">
+      <c r="T8" s="5">
         <v>0.16011785000000001</v>
       </c>
-      <c r="U8" s="6">
+      <c r="U8" s="5">
         <v>0.17114433000000001</v>
       </c>
-      <c r="V8" s="6">
+      <c r="V8" s="5">
         <v>0.13993164999999999</v>
       </c>
     </row>
@@ -961,31 +983,31 @@
       <c r="L10" s="2">
         <v>2.1626186636007259E-2</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="5">
         <v>0.37513227999999998</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="5">
         <v>0.35283505999999998</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="5">
         <v>0.16536479000000001</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="5">
         <v>0.34285968999999999</v>
       </c>
-      <c r="R10" s="6">
+      <c r="R10" s="5">
         <v>4.7619000000000003E-3</v>
       </c>
-      <c r="S10" s="6">
+      <c r="S10" s="5">
         <v>0.18555556000000001</v>
       </c>
-      <c r="T10" s="6">
+      <c r="T10" s="5">
         <v>6.0317460000000003E-2</v>
       </c>
-      <c r="U10" s="6">
+      <c r="U10" s="5">
         <v>0.23990232</v>
       </c>
-      <c r="V10" s="6">
+      <c r="V10" s="5">
         <v>0.16560847000000001</v>
       </c>
     </row>
@@ -1064,16 +1086,16 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="N15" s="5"/>
+      <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="N16" s="5"/>
+      <c r="N16" s="4"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="N17" s="5"/>
+      <c r="N17" s="4"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="2">
@@ -1103,10 +1125,10 @@
       <c r="L18" s="2">
         <v>8.7485354274540489E-2</v>
       </c>
-      <c r="N18" s="5"/>
+      <c r="N18" s="4"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="2">
@@ -1136,10 +1158,10 @@
       <c r="L19" s="2">
         <v>0.1861747296935245</v>
       </c>
-      <c r="N19" s="5"/>
+      <c r="N19" s="4"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="2">
@@ -1178,28 +1200,28 @@
         <f t="shared" si="2"/>
         <v>0.11903498638190504</v>
       </c>
-      <c r="N20" s="5"/>
+      <c r="N20" s="4"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="N21" s="5"/>
+      <c r="N21" s="4"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="N22" s="5"/>
+      <c r="N22" s="4"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="N23" s="5"/>
+      <c r="N23" s="4"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="N24" s="5"/>
+      <c r="N24" s="4"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="N25" s="5"/>
+      <c r="N25" s="4"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="N26" s="5"/>
+      <c r="N26" s="4"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="N27" s="5"/>
+      <c r="N27" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1209,4 +1231,747 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543A9E21-8676-454E-8886-AC1E8BC656F1}">
+  <dimension ref="A1:AE20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="D1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="W1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="W3" s="2">
+        <v>0.35967883</v>
+      </c>
+      <c r="X3" s="2">
+        <v>9.1129370000000001E-2</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>0.32926939999999999</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>0.16213610000000001</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>0.14394483999999999</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>0.30428157</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>0.18831534999999999</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>0.24454435999999999</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>0.29820143999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7">
+        <v>8036</v>
+      </c>
+      <c r="C4" s="7">
+        <v>345900</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.16878927525184845</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.5687876264950702E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5.0530312551085581E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.17108473359180318</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.17026508017778103</v>
+      </c>
+      <c r="I4" s="2">
+        <v>7.481713967032895E-2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.69186867034762423</v>
+      </c>
+      <c r="K4" s="2">
+        <v>5.8312715640325367E-3</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.1114989387056555</v>
+      </c>
+      <c r="M4" s="2">
+        <v>5.7144140633121135E-2</v>
+      </c>
+      <c r="N4" s="2">
+        <v>5.5578463432355785E-2</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.12253802456657856</v>
+      </c>
+      <c r="W4" s="2">
+        <v>0.36808990000000003</v>
+      </c>
+      <c r="X4" s="2">
+        <v>4.538416E-2</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>0.15184650999999999</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>0.48207327</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>1.9327049999999998E-2</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>0.21238736</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>6.6743979999999994E-2</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>7.8925220000000004E-2</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>0.21247477000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="W5" s="5">
+        <v>0.34246383000000002</v>
+      </c>
+      <c r="X5" s="5">
+        <v>0.16423603000000001</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>0.24050800999999999</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>0.16705046000000001</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>6.1724910000000001E-2</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>0.17220925000000001</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>0.25656886000000001</v>
+      </c>
+      <c r="AD5" s="5">
+        <v>0.26182491000000002</v>
+      </c>
+      <c r="AE5" s="5">
+        <v>0.16842712000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7">
+        <v>644</v>
+      </c>
+      <c r="C6" s="7">
+        <v>2523</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.18078032216230974</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3.9739655616984774E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.1373074173928211</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.45972005263542531</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.25818808624728468</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.16423054171501378</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.22651259874659246</v>
+      </c>
+      <c r="K6" s="2">
+        <v>3.7707039337474109E-2</v>
+      </c>
+      <c r="L6" s="2">
+        <v>8.1146622528610102E-2</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.35837155641115281</v>
+      </c>
+      <c r="N6" s="2">
+        <v>5.6832298136645962E-2</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.11264646326758129</v>
+      </c>
+      <c r="W6" s="5">
+        <v>0.19669489000000001</v>
+      </c>
+      <c r="X6" s="5">
+        <v>9.5825530000000006E-2</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>0.1803826</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>0.12524266000000001</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>4.1971370000000001E-2</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>0.10716726</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>0.18308652</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>4.329028E-2</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>0.13776347999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="W8" s="5">
+        <v>0.21877938999999999</v>
+      </c>
+      <c r="X8" s="5">
+        <v>0.10597388000000001</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>0.19811214999999999</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>9.0702859999999996E-2</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>4.2192130000000001E-2</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>0.1597181</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>0.16011785000000001</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>0.17114433000000001</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>0.13993164999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="7">
+        <v>2484</v>
+      </c>
+      <c r="C10" s="7">
+        <v>75616</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.11424332216519706</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.100960704829317</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.13668760426310811</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.41927277706046184</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.31265817709648752</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5.5587250477982311E-2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.56693264965875456</v>
+      </c>
+      <c r="K10" s="2">
+        <v>4.830917874396135E-3</v>
+      </c>
+      <c r="L10" s="2">
+        <v>7.1482777510911255E-2</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2.3953015718796124E-2</v>
+      </c>
+      <c r="N10" s="2">
+        <v>7.7852321930573634E-2</v>
+      </c>
+      <c r="O10" s="2">
+        <v>3.8719753668914489E-2</v>
+      </c>
+      <c r="W10" s="5">
+        <v>0.37513227999999998</v>
+      </c>
+      <c r="X10" s="5">
+        <v>0.35283505999999998</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>0.16536479000000001</v>
+      </c>
+      <c r="Z10" s="5">
+        <v>0.34285968999999999</v>
+      </c>
+      <c r="AA10" s="5">
+        <v>4.7619000000000003E-3</v>
+      </c>
+      <c r="AB10" s="5">
+        <v>0.18555556000000001</v>
+      </c>
+      <c r="AC10" s="5">
+        <v>6.0317460000000003E-2</v>
+      </c>
+      <c r="AD10" s="5">
+        <v>0.23990232</v>
+      </c>
+      <c r="AE10" s="5">
+        <v>0.16560847000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="D11" s="2">
+        <f>(D3*2780+D4*8116+D5*4382+D6*672+D8*7857+D10*2492)/26299</f>
+        <v>6.7533841335136138E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" ref="E11:L11" si="0">(E3*2780+E4*8116+E5*4382+E6*672+E8*7857+E10*2492)/26299</f>
+        <v>1.8509522368744501E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>3.2054454959361642E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10427329303915553</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>8.8768316742290326E-2</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="0"/>
+        <v>3.2552654389444886E-2</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.2730225011539848</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="0"/>
+        <v>3.2208212400268391E-3</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="0"/>
+        <v>4.3256055303681394E-2</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="W11" s="2">
+        <f>(W3*2780+W4*8116+W5*4382+W6*672+W8*7857+W10*2492)/26299</f>
+        <v>0.31461118498536067</v>
+      </c>
+      <c r="X11" s="2">
+        <f t="shared" ref="X11:AE11" si="1">(X3*2780+X4*8116+X5*4382+X6*672+X8*7857+X10*2492)/26299</f>
+        <v>0.11854657117989277</v>
+      </c>
+      <c r="Y11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.20120668593520663</v>
+      </c>
+      <c r="Z11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25652997905091446</v>
+      </c>
+      <c r="AA11" s="2">
+        <f t="shared" si="1"/>
+        <v>4.559407313852238E-2</v>
+      </c>
+      <c r="AB11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.19444030106848167</v>
+      </c>
+      <c r="AC11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14148396358834936</v>
+      </c>
+      <c r="AD11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16880169635157233</v>
+      </c>
+      <c r="AE11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.1861747296935245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.1529475040784378</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.41289294285969352</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.10471706598334657</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.47923490790981721</v>
+      </c>
+      <c r="H18" s="2">
+        <v>2.2923072389783618E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>9.3623570934537145E-2</v>
+      </c>
+      <c r="J18" s="2">
+        <v>8.3791634451571229E-2</v>
+      </c>
+      <c r="K18" s="2">
+        <v>8.1541894730175465E-2</v>
+      </c>
+      <c r="L18" s="2">
+        <v>8.7485354274540489E-2</v>
+      </c>
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C19" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.31461118498536067</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.11854657117989277</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.20120668593520663</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.25652997905091446</v>
+      </c>
+      <c r="H19" s="2">
+        <v>4.559407313852238E-2</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.19444030106848167</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.14148396358834936</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.16880169635157233</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.1861747296935245</v>
+      </c>
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C20" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="2">
+        <f>(2*D18*D19)/(D18+D19)</f>
+        <v>0.20583082562328234</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" ref="E20:L20" si="2">(2*E18*E19)/(E18+E19)</f>
+        <v>0.18420550729596688</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="2"/>
+        <v>0.13774526283253077</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="2"/>
+        <v>0.33417773276569429</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="2"/>
+        <v>3.0507874519310189E-2</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="2"/>
+        <v>0.12638999255989294</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="2"/>
+        <v>0.1052503925050378</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="2"/>
+        <v>0.10996415042780378</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="2"/>
+        <v>0.11903498638190504</v>
+      </c>
+      <c r="N20" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="W1:AE1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the reporting, implemented Query generation for python, updated Cochange calculation process in java, manually merged lab pc with local pc. I found some files are lost in earlier push or pull operation :(
</commit_message>
<xml_diff>
--- a/data_files/final_dataset_jss/processed_result.xlsx
+++ b/data_files/final_dataset_jss/processed_result.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdn769\FindCochangeByClone\data_files\final_dataset_jss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE24ACD1-65AF-40FE-A9C6-71519B79F9C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC73231E-909D-4730-B568-304739AAA6CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-4404" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Result" sheetId="1" r:id="rId1"/>
     <sheet name="cw_separate_types" sheetId="2" r:id="rId2"/>
+    <sheet name="max cochange" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
   <si>
     <t>ccfinder</t>
   </si>
@@ -115,6 +116,18 @@
   </si>
   <si>
     <t>cw_type3token</t>
+  </si>
+  <si>
+    <t>Determine Maximum number of cochange with a seed change (Which clone detection tool?)</t>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>Tools</t>
   </si>
 </sst>
 </file>
@@ -158,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -184,6 +197,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -469,7 +485,7 @@
   <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:V20"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,28 +506,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="N1" s="8" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="N1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -1235,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543A9E21-8676-454E-8886-AC1E8BC656F1}">
-  <dimension ref="A1:AE20"/>
+  <dimension ref="A1:AB40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1257,49 +1273,43 @@
     <col min="12" max="12" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="13" max="15" width="12" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="8.88671875" style="7"/>
+    <col min="17" max="17" width="7.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="D1" s="8" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="D1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="W1" s="8" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="Q1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
@@ -1342,338 +1352,542 @@
       <c r="O2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="Q2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="X2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="7" t="s">
+      <c r="R2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="W2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="X2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="Y2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="Z2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AD2" s="7" t="s">
+      <c r="AA2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AE2" s="7" t="s">
+      <c r="AB2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="W3" s="2">
-        <v>0.35967883</v>
-      </c>
-      <c r="X3" s="2">
-        <v>9.1129370000000001E-2</v>
-      </c>
-      <c r="Y3" s="2">
-        <v>0.32926939999999999</v>
-      </c>
-      <c r="Z3" s="2">
-        <v>0.16213610000000001</v>
-      </c>
-      <c r="AA3" s="2">
-        <v>0.14394483999999999</v>
-      </c>
-      <c r="AB3" s="2">
-        <v>0.30428157</v>
-      </c>
-      <c r="AC3" s="2">
-        <v>0.18831534999999999</v>
-      </c>
-      <c r="AD3" s="2">
-        <v>0.24454435999999999</v>
-      </c>
-      <c r="AE3" s="2">
-        <v>0.29820143999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B3" s="7">
+        <v>2909</v>
+      </c>
+      <c r="C3" s="7">
+        <v>33578</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.26128887512390214</v>
+      </c>
+      <c r="E3" s="2">
+        <v>6.6502573992728964E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.1001653605223721</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.42996072770301946</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.2213799883507718</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.25964507989095897</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.23890011959553353</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.10352213342253866</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.23530983229584282</v>
+      </c>
+      <c r="M3" s="2">
+        <v>9.3817886798157168E-2</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0.12770922931680292</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.21870288872736493</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>0.34372881999999999</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0.15795795000000001</v>
+      </c>
+      <c r="S3" s="5">
+        <v>0.20241644</v>
+      </c>
+      <c r="T3" s="5">
+        <v>0.25003483999999998</v>
+      </c>
+      <c r="U3" s="5">
+        <v>0.35201194000000002</v>
+      </c>
+      <c r="V3" s="5">
+        <v>0.3146679</v>
+      </c>
+      <c r="W3" s="5">
+        <v>0.15494615</v>
+      </c>
+      <c r="X3" s="5">
+        <v>0.13756159000000001</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>0.29078817000000001</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>0.17996448000000001</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>0.23370001000000001</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>0.28497766000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="7">
-        <v>8036</v>
+        <v>8052</v>
       </c>
       <c r="C4" s="7">
-        <v>345900</v>
+        <v>346140</v>
       </c>
       <c r="D4" s="2">
-        <v>0.16878927525184845</v>
+        <v>0.1683433270549558</v>
       </c>
       <c r="E4" s="2">
-        <v>2.5687876264950702E-2</v>
+        <v>2.5576372641884504E-2</v>
       </c>
       <c r="F4" s="2">
-        <v>5.0530312551085581E-2</v>
+        <v>5.2017521705816978E-2</v>
       </c>
       <c r="G4" s="2">
-        <v>0.17108473359180318</v>
+        <v>0.1745850628112704</v>
       </c>
       <c r="H4" s="2">
-        <v>0.17026508017778103</v>
+        <v>0.17527980319730138</v>
       </c>
       <c r="I4" s="2">
-        <v>7.481713967032895E-2</v>
+        <v>7.460522438898233E-2</v>
       </c>
       <c r="J4" s="2">
-        <v>0.69186867034762423</v>
+        <v>0.68955044535439758</v>
       </c>
       <c r="K4" s="2">
-        <v>5.8312715640325367E-3</v>
+        <v>5.8188483744716912E-3</v>
       </c>
       <c r="L4" s="2">
-        <v>0.1114989387056555</v>
+        <v>0.11117439660966945</v>
       </c>
       <c r="M4" s="2">
-        <v>5.7144140633121135E-2</v>
+        <v>5.6843510951151636E-2</v>
       </c>
       <c r="N4" s="2">
-        <v>5.5578463432355785E-2</v>
+        <v>5.5349745552661464E-2</v>
       </c>
       <c r="O4" s="2">
-        <v>0.12253802456657856</v>
-      </c>
-      <c r="W4" s="2">
-        <v>0.36808990000000003</v>
-      </c>
-      <c r="X4" s="2">
-        <v>4.538416E-2</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>0.15184650999999999</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>0.48207327</v>
-      </c>
-      <c r="AA4" s="2">
-        <v>1.9327049999999998E-2</v>
-      </c>
-      <c r="AB4" s="2">
-        <v>0.21238736</v>
-      </c>
-      <c r="AC4" s="2">
-        <v>6.6743979999999994E-2</v>
-      </c>
-      <c r="AD4" s="2">
-        <v>7.8925220000000004E-2</v>
-      </c>
-      <c r="AE4" s="2">
-        <v>0.21247477000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+        <v>0.12220086961858032</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0.37099252999999999</v>
+      </c>
+      <c r="R4" s="5">
+        <v>5.7638189999999999E-2</v>
+      </c>
+      <c r="S4" s="5">
+        <v>9.3283809999999995E-2</v>
+      </c>
+      <c r="T4" s="5">
+        <v>0.15123865</v>
+      </c>
+      <c r="U4" s="5">
+        <v>0.1820708</v>
+      </c>
+      <c r="V4" s="5">
+        <v>0.15304392</v>
+      </c>
+      <c r="W4" s="5">
+        <v>0.48587472999999998</v>
+      </c>
+      <c r="X4" s="5">
+        <v>1.9479449999999999E-2</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>0.21406217</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>6.7270300000000005E-2</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>7.9547590000000001E-2</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>0.21415027</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="B5" s="7">
+        <v>4582</v>
+      </c>
+      <c r="C5" s="7">
+        <v>254311</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.1401173161994029</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3.5063820862266726E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.17194790586675388</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.60401997810108476</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.22915798438937657</v>
+      </c>
+      <c r="I5" s="2">
+        <v>8.135538361452016E-2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.30579862696362087</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.1044663330818409E-2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>5.376010606571182E-2</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.11662991199892592</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.10733313126412175</v>
+      </c>
+      <c r="O5" s="2">
+        <v>4.066622121678775E-2</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0.32751560000000002</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0.17536930000000001</v>
+      </c>
+      <c r="S5" s="5">
+        <v>0.29288862999999998</v>
+      </c>
+      <c r="T5" s="5">
+        <v>0.25724190000000002</v>
+      </c>
+      <c r="U5" s="5">
+        <v>0.39727678</v>
+      </c>
+      <c r="V5" s="5">
+        <v>0.23001005999999999</v>
+      </c>
       <c r="W5" s="5">
-        <v>0.34246383000000002</v>
+        <v>0.15975887</v>
       </c>
       <c r="X5" s="5">
-        <v>0.16423603000000001</v>
+        <v>5.9030680000000002E-2</v>
       </c>
       <c r="Y5" s="5">
-        <v>0.24050800999999999</v>
+        <v>0.16469248</v>
       </c>
       <c r="Z5" s="5">
-        <v>0.16705046000000001</v>
+        <v>0.24536986999999999</v>
       </c>
       <c r="AA5" s="5">
-        <v>6.1724910000000001E-2</v>
+        <v>0.25039650000000002</v>
       </c>
       <c r="AB5" s="5">
-        <v>0.17220925000000001</v>
-      </c>
-      <c r="AC5" s="5">
-        <v>0.25656886000000001</v>
-      </c>
-      <c r="AD5" s="5">
-        <v>0.26182491000000002</v>
-      </c>
-      <c r="AE5" s="5">
-        <v>0.16842712000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+        <v>0.16107542999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="7">
-        <v>644</v>
+        <v>718</v>
       </c>
       <c r="C6" s="7">
-        <v>2523</v>
+        <v>3648</v>
       </c>
       <c r="D6" s="2">
-        <v>0.18078032216230974</v>
+        <v>0.14857443655985367</v>
       </c>
       <c r="E6" s="2">
-        <v>3.9739655616984774E-2</v>
+        <v>2.1342921238464391E-2</v>
       </c>
       <c r="F6" s="2">
-        <v>0.1373074173928211</v>
+        <v>9.9084241695457487E-2</v>
       </c>
       <c r="G6" s="2">
-        <v>0.45972005263542531</v>
+        <v>0.60747947670861591</v>
       </c>
       <c r="H6" s="2">
-        <v>0.25818808624728468</v>
+        <v>0.22764930120188728</v>
       </c>
       <c r="I6" s="2">
-        <v>0.16423054171501378</v>
+        <v>0.13204761380044039</v>
       </c>
       <c r="J6" s="2">
-        <v>0.22651259874659246</v>
+        <v>0.19532384318811893</v>
       </c>
       <c r="K6" s="2">
-        <v>3.7707039337474109E-2</v>
+        <v>2.831608966706458E-2</v>
       </c>
       <c r="L6" s="2">
-        <v>8.1146622528610102E-2</v>
+        <v>6.8264596746490894E-2</v>
       </c>
       <c r="M6" s="2">
-        <v>0.35837155641115281</v>
+        <v>0.2614702883412941</v>
       </c>
       <c r="N6" s="2">
-        <v>5.6832298136645962E-2</v>
+        <v>4.8726621567847198E-2</v>
       </c>
       <c r="O6" s="2">
-        <v>0.11264646326758129</v>
+        <v>9.2856505147591514E-2</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0.18409327</v>
+      </c>
+      <c r="R6" s="5">
+        <v>5.1887240000000001E-2</v>
+      </c>
+      <c r="S6" s="5">
+        <v>0.14710994999999999</v>
+      </c>
+      <c r="T6" s="5">
+        <v>0.15424735000000001</v>
+      </c>
+      <c r="U6" s="5">
+        <v>0.24713941</v>
+      </c>
+      <c r="V6" s="5">
+        <v>0.16882606</v>
       </c>
       <c r="W6" s="5">
-        <v>0.19669489000000001</v>
+        <v>0.11721876000000001</v>
       </c>
       <c r="X6" s="5">
-        <v>9.5825530000000006E-2</v>
+        <v>3.9282400000000002E-2</v>
       </c>
       <c r="Y6" s="5">
-        <v>0.1803826</v>
+        <v>0.10030139</v>
       </c>
       <c r="Z6" s="5">
-        <v>0.12524266000000001</v>
+        <v>0.17135674000000001</v>
       </c>
       <c r="AA6" s="5">
-        <v>4.1971370000000001E-2</v>
+        <v>4.051681E-2</v>
       </c>
       <c r="AB6" s="5">
-        <v>0.10716726</v>
-      </c>
-      <c r="AC6" s="5">
-        <v>0.18308652</v>
-      </c>
-      <c r="AD6" s="5">
-        <v>4.329028E-2</v>
-      </c>
-      <c r="AE6" s="5">
-        <v>0.13776347999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+        <v>0.12893740000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
+        <v>6865</v>
+      </c>
+      <c r="C7" s="7">
+        <v>265213</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6.3605696000000003E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2.1374997999999999E-2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>7.8849591999999996E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.34723603400000003</v>
+      </c>
+      <c r="H7" s="2">
+        <v>8.6439531E-2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>5.8612012999999998E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.59716882599999999</v>
+      </c>
+      <c r="K7" s="2">
+        <v>8.0654239999999999E-3</v>
+      </c>
+      <c r="L7" s="2">
+        <v>2.3638247000000001E-2</v>
+      </c>
+      <c r="M7" s="2">
+        <v>2.8282055E-2</v>
+      </c>
+      <c r="N7" s="2">
+        <v>3.4404730000000001E-2</v>
+      </c>
+      <c r="O7" s="2">
+        <v>2.0560788E-2</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0.13800519999999999</v>
+      </c>
+      <c r="R7" s="5">
+        <v>5.1237400000000002E-2</v>
+      </c>
+      <c r="S7" s="5">
+        <v>8.9317480000000005E-2</v>
+      </c>
+      <c r="T7" s="5">
+        <v>9.2134740000000007E-2</v>
+      </c>
+      <c r="U7" s="5">
+        <v>0.14704138999999999</v>
+      </c>
+      <c r="V7" s="5">
+        <v>0.10524989</v>
+      </c>
+      <c r="W7" s="5">
+        <v>0.19862555000000001</v>
+      </c>
+      <c r="X7" s="5">
+        <v>1.6958000000000001E-2</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>4.4279590000000001E-2</v>
+      </c>
+      <c r="Z7" s="5">
+        <v>4.8073310000000001E-2</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>7.1806339999999996E-2</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>4.8562599999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="B8" s="7">
+        <v>8313</v>
+      </c>
+      <c r="C8" s="7">
+        <v>455469</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.11319835981612518</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3.064367716838938E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.10126647314409529</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.52042422259876187</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.15480653096138733</v>
+      </c>
+      <c r="I8" s="2">
+        <v>8.9959841748021172E-2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.386597186829578</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1.5972289531560543E-2</v>
+      </c>
+      <c r="L8" s="2">
+        <v>6.139685044544612E-2</v>
+      </c>
+      <c r="M8" s="2">
+        <v>7.9230793482322814E-2</v>
+      </c>
+      <c r="N8" s="2">
+        <v>7.2549324534107007E-2</v>
+      </c>
+      <c r="O8" s="2">
+        <v>4.6066254660553516E-2</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>0.2067785</v>
+      </c>
+      <c r="R8" s="5">
+        <v>0.10091334</v>
+      </c>
+      <c r="S8" s="5">
+        <v>0.17041735999999999</v>
+      </c>
+      <c r="T8" s="5">
+        <v>0.21528511</v>
+      </c>
+      <c r="U8" s="5">
+        <v>0.28800847000000002</v>
+      </c>
+      <c r="V8" s="5">
+        <v>0.18724494</v>
+      </c>
       <c r="W8" s="5">
-        <v>0.21877938999999999</v>
+        <v>8.5727460000000005E-2</v>
       </c>
       <c r="X8" s="5">
-        <v>0.10597388000000001</v>
+        <v>3.987773E-2</v>
       </c>
       <c r="Y8" s="5">
-        <v>0.19811214999999999</v>
+        <v>0.15095695000000001</v>
       </c>
       <c r="Z8" s="5">
-        <v>9.0702859999999996E-2</v>
+        <v>0.15133477000000001</v>
       </c>
       <c r="AA8" s="5">
-        <v>4.2192130000000001E-2</v>
+        <v>0.16175639999999999</v>
       </c>
       <c r="AB8" s="5">
-        <v>0.1597181</v>
-      </c>
-      <c r="AC8" s="5">
-        <v>0.16011785000000001</v>
-      </c>
-      <c r="AD8" s="5">
-        <v>0.17114433000000001</v>
-      </c>
-      <c r="AE8" s="5">
-        <v>0.13993164999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+        <v>0.13225586</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
@@ -1689,210 +1903,278 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="7">
-        <v>2484</v>
+        <v>2508</v>
       </c>
       <c r="C10" s="7">
-        <v>75616</v>
+        <v>97396</v>
       </c>
       <c r="D10" s="2">
-        <v>0.11424332216519706</v>
+        <v>0.1054961160521711</v>
       </c>
       <c r="E10" s="2">
-        <v>0.100960704829317</v>
+        <v>7.56835729174863E-2</v>
       </c>
       <c r="F10" s="2">
-        <v>0.13668760426310811</v>
+        <v>0.11233215045429397</v>
       </c>
       <c r="G10" s="2">
-        <v>0.41927277706046184</v>
+        <v>0.50104182992018786</v>
       </c>
       <c r="H10" s="2">
-        <v>0.31265817709648752</v>
+        <v>0.32756816462582083</v>
       </c>
       <c r="I10" s="2">
-        <v>5.5587250477982311E-2</v>
+        <v>5.0066456251550172E-2</v>
       </c>
       <c r="J10" s="2">
-        <v>0.56693264965875456</v>
+        <v>0.50518975920166476</v>
       </c>
       <c r="K10" s="2">
-        <v>4.830917874396135E-3</v>
+        <v>4.7846889952153108E-3</v>
       </c>
       <c r="L10" s="2">
-        <v>7.1482777510911255E-2</v>
+        <v>6.5596874850248704E-2</v>
       </c>
       <c r="M10" s="2">
-        <v>2.3953015718796124E-2</v>
+        <v>2.0165847517132858E-2</v>
       </c>
       <c r="N10" s="2">
-        <v>7.7852321930573634E-2</v>
+        <v>6.1271956632230472E-2</v>
       </c>
       <c r="O10" s="2">
-        <v>3.8719753668914489E-2</v>
+        <v>3.4205709129131311E-2</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0.37276551000000002</v>
+      </c>
+      <c r="R10" s="5">
+        <v>0.21184937000000001</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0.33582014999999998</v>
+      </c>
+      <c r="T10" s="5">
+        <v>0.4749023</v>
+      </c>
+      <c r="U10" s="5">
+        <v>0.59375186999999996</v>
+      </c>
+      <c r="V10" s="5">
+        <v>0.16432147999999999</v>
       </c>
       <c r="W10" s="5">
-        <v>0.37513227999999998</v>
+        <v>0.34069653999999999</v>
       </c>
       <c r="X10" s="5">
-        <v>0.35283505999999998</v>
+        <v>4.7318600000000001E-3</v>
       </c>
       <c r="Y10" s="5">
-        <v>0.16536479000000001</v>
+        <v>0.18438486000000001</v>
       </c>
       <c r="Z10" s="5">
-        <v>0.34285968999999999</v>
+        <v>5.9936910000000003E-2</v>
       </c>
       <c r="AA10" s="5">
-        <v>4.7619000000000003E-3</v>
+        <v>0.23838873999999999</v>
       </c>
       <c r="AB10" s="5">
-        <v>0.18555556000000001</v>
-      </c>
-      <c r="AC10" s="5">
-        <v>6.0317460000000003E-2</v>
-      </c>
-      <c r="AD10" s="5">
-        <v>0.23990232</v>
-      </c>
-      <c r="AE10" s="5">
-        <v>0.16560847000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+        <v>0.16456361999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D11" s="2">
-        <f>(D3*2780+D4*8116+D5*4382+D6*672+D8*7857+D10*2492)/26299</f>
-        <v>6.7533841335136138E-2</v>
+        <f>(D3*2909+D4*8052+D5*4582+D6*718+D7*6865+D8*8313+D10*2508)/27082</f>
+        <v>0.16640348285606194</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" ref="E11:L11" si="0">(E3*2780+E4*8116+E5*4382+E6*672+E8*7857+E10*2492)/26299</f>
-        <v>1.8509522368744501E-2</v>
+        <f>(E3*2909+E4*8052+E5*4582+E6*718+E7*6865+E8*8313+E10*2508)/27082</f>
+        <v>4.3079471063632781E-2</v>
       </c>
       <c r="F11" s="2">
+        <f>(F3*2909+F4*8052+F5*4582+F6*718+F7*6865+F8*8313+F10*2508)/27082</f>
+        <v>0.11941856518794243</v>
+      </c>
+      <c r="G11" s="2">
+        <f>(G3*2909+G4*8052+G5*4582+G6*718+G7*6865+G8*8313+G10*2508)/27082</f>
+        <v>0.5105597567348692</v>
+      </c>
+      <c r="H11" s="2">
+        <f>(H3*2909+H4*8052+H5*4582+H6*718+H7*6865+H8*8313+H10*2508)/27082</f>
+        <v>0.22046586194781462</v>
+      </c>
+      <c r="I11" s="2">
+        <f>(I3*2909+I4*8052+I5*4582+I6*718+I7*6865+I8*8313+I10*2508)/27082</f>
+        <v>0.11444441564834654</v>
+      </c>
+      <c r="J11" s="2">
+        <f>(J3*2909+J4*8052+J5*4582+J6*718+J7*6865+J8*8313+J10*2508)/27082</f>
+        <v>0.6044234097457889</v>
+      </c>
+      <c r="K11" s="2">
+        <f>(K3*2909+K4*8052+K5*4582+K6*718+K7*6865+K8*8313+K10*2508)/27082</f>
+        <v>2.4551496626395251E-2</v>
+      </c>
+      <c r="L11" s="2">
+        <f>(L3*2909+L4*8052+L5*4582+L6*718+L7*6865+L8*8313+L10*2508)/27082</f>
+        <v>0.1001484704098351</v>
+      </c>
+      <c r="M11" s="2">
+        <f>(M3*2909+M4*8052+M5*4582+M6*718+M7*6865+M8*8313+M10*2508)/27082</f>
+        <v>8.6999924158081346E-2</v>
+      </c>
+      <c r="N11" s="2">
+        <f>(N3*2909+N4*8052+N5*4582+N6*718+N7*6865+N8*8313+N10*2508)/27082</f>
+        <v>8.6290875657122651E-2</v>
+      </c>
+      <c r="O11" s="2">
+        <f>(O3*2909+O4*8052+O5*4582+O6*718+O7*6865+O8*8313+O10*2508)/27082</f>
+        <v>9.1686662908834218E-2</v>
+      </c>
+      <c r="Q11" s="2">
+        <f>(Q3*2909+Q4*8052+Q5*4582+Q6*718+Q7*6865+Q8*8313+Q10*2508)/27082</f>
+        <v>0.34049352719813897</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" ref="R11:AB11" si="0">(R3*2909+R4*8052+R5*4582+R6*718+R7*6865+R8*8313+R10*2508)/27082</f>
+        <v>0.12873329590613694</v>
+      </c>
+      <c r="S11" s="2">
         <f t="shared" si="0"/>
-        <v>3.2054454959361642E-2</v>
-      </c>
-      <c r="G11" s="2">
+        <v>0.2089828025596337</v>
+      </c>
+      <c r="T11" s="2">
         <f t="shared" si="0"/>
-        <v>0.10427329303915553</v>
-      </c>
-      <c r="H11" s="2">
+        <v>0.25285363047005394</v>
+      </c>
+      <c r="U11" s="2">
         <f t="shared" si="0"/>
-        <v>8.8768316742290326E-2</v>
-      </c>
-      <c r="I11" s="2">
+        <v>0.34637723804815007</v>
+      </c>
+      <c r="V11" s="2">
         <f t="shared" si="0"/>
-        <v>3.2552654389444886E-2</v>
-      </c>
-      <c r="J11" s="2">
+        <v>0.22206734081123991</v>
+      </c>
+      <c r="W11" s="2">
         <f t="shared" si="0"/>
-        <v>0.2730225011539848</v>
-      </c>
-      <c r="K11" s="2">
+        <v>0.29945585947788195</v>
+      </c>
+      <c r="X11" s="2">
         <f t="shared" si="0"/>
-        <v>3.2208212400268391E-3</v>
-      </c>
-      <c r="L11" s="2">
+        <v>4.8574192454028511E-2</v>
+      </c>
+      <c r="Y11" s="2">
         <f t="shared" si="0"/>
-        <v>4.3256055303681394E-2</v>
-      </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="W11" s="2">
-        <f>(W3*2780+W4*8116+W5*4382+W6*672+W8*7857+W10*2492)/26299</f>
-        <v>0.31461118498536067</v>
-      </c>
-      <c r="X11" s="2">
-        <f t="shared" ref="X11:AE11" si="1">(X3*2780+X4*8116+X5*4382+X6*672+X8*7857+X10*2492)/26299</f>
-        <v>0.11854657117989277</v>
-      </c>
-      <c r="Y11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.20120668593520663</v>
+        <v>0.20004026513292963</v>
       </c>
       <c r="Z11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.25652997905091446</v>
+        <f t="shared" si="0"/>
+        <v>0.14957857610294659</v>
       </c>
       <c r="AA11" s="2">
-        <f t="shared" si="1"/>
-        <v>4.559407313852238E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.18212350615057971</v>
       </c>
       <c r="AB11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.19444030106848167</v>
-      </c>
-      <c r="AC11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.14148396358834936</v>
-      </c>
-      <c r="AD11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.16880169635157233</v>
-      </c>
-      <c r="AE11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.1861747296935245</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>0.19309923316520197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="N15" s="9"/>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="R15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="S15" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="N16" s="9"/>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="R16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0.35280720740855737</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
       <c r="N17" s="9"/>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="R17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S17" s="2">
+        <v>0.31665799211299567</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="C18" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="2">
-        <v>0.1529475040784378</v>
+        <v>0.15028011297791405</v>
       </c>
       <c r="E18" s="2">
-        <v>0.41289294285969352</v>
+        <v>3.766113559099412E-2</v>
       </c>
       <c r="F18" s="2">
-        <v>0.10471706598334657</v>
+        <v>9.9431029220140937E-2</v>
       </c>
       <c r="G18" s="2">
-        <v>0.47923490790981721</v>
+        <v>0.42253910193057115</v>
       </c>
       <c r="H18" s="2">
-        <v>2.2923072389783618E-2</v>
+        <v>0.19855435687747269</v>
       </c>
       <c r="I18" s="2">
-        <v>9.3623570934537145E-2</v>
+        <v>9.9586891490418744E-2</v>
       </c>
       <c r="J18" s="2">
-        <v>8.3791634451571229E-2</v>
+        <v>0.45304744081845705</v>
       </c>
       <c r="K18" s="2">
-        <v>8.1541894730175465E-2</v>
+        <v>2.2506997115280855E-2</v>
       </c>
       <c r="L18" s="2">
-        <v>8.7485354274540489E-2</v>
-      </c>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
+        <v>9.4156425300352786E-2</v>
+      </c>
+      <c r="M18" s="2">
+        <v>7.9830722933097967E-2</v>
+      </c>
+      <c r="N18" s="2">
+        <v>7.7569641204349588E-2</v>
+      </c>
+      <c r="O18" s="2">
+        <v>8.6474721042650041E-2</v>
+      </c>
+      <c r="R18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S18" s="2">
+        <v>0.25736684309358249</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C19" s="10" t="s">
         <v>21</v>
       </c>
@@ -1924,54 +2206,321 @@
         <v>0.1861747296935245</v>
       </c>
       <c r="N19" s="9"/>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="R19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="S19" s="2">
+        <v>0.21545460883405504</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C20" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="2">
         <f>(2*D18*D19)/(D18+D19)</f>
-        <v>0.20583082562328234</v>
+        <v>0.20340154625759593</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" ref="E20:L20" si="2">(2*E18*E19)/(E18+E19)</f>
-        <v>0.18420550729596688</v>
+        <f>(2*E18*E19)/(E18+E19)</f>
+        <v>5.7162333195271829E-2</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="2"/>
-        <v>0.13774526283253077</v>
+        <f>(2*F18*F19)/(F18+F19)</f>
+        <v>0.13309167053889776</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="2"/>
-        <v>0.33417773276569429</v>
+        <f>(2*G18*G19)/(G18+G19)</f>
+        <v>0.31924276926222445</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="2"/>
-        <v>3.0507874519310189E-2</v>
+        <f>(2*H18*H19)/(H18+H19)</f>
+        <v>7.4159001299747659E-2</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="2"/>
-        <v>0.12638999255989294</v>
+        <f>(2*I18*I19)/(I18+I19)</f>
+        <v>0.13171370304460694</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="2"/>
-        <v>0.1052503925050378</v>
+        <f>(2*J18*J19)/(J18+J19)</f>
+        <v>0.2156284668747083</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="2"/>
-        <v>0.10996415042780378</v>
+        <f>(2*K18*K19)/(K18+K19)</f>
+        <v>3.9718208555928683E-2</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="2"/>
-        <v>0.11903498638190504</v>
+        <f>(2*L18*L19)/(L18+L19)</f>
+        <v>0.12506313848408732</v>
       </c>
       <c r="N20" s="9"/>
+      <c r="R20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="S20" s="2">
+        <v>0.14555626850919298</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="R21" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S21" s="2">
+        <v>0.1443428629641893</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="R22" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S22" s="2">
+        <v>0.13087857231531486</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="R23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="S23" s="2">
+        <v>0.12166917144513506</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="R24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S24" s="2">
+        <v>0.11306335716411227</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.16640348274325442</v>
+      </c>
+      <c r="E25" s="2">
+        <v>4.3079471059581161E-2</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.11941856530437982</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.51055975668652631</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.22046586187181957</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.11444441562980644</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.60442340962375296</v>
+      </c>
+      <c r="K25" s="2">
+        <v>2.4551496715014557E-2</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.10014847038789471</v>
+      </c>
+      <c r="M25" s="2">
+        <v>8.6999924243698012E-2</v>
+      </c>
+      <c r="N25" s="2">
+        <v>8.6290875586467419E-2</v>
+      </c>
+      <c r="O25" s="2">
+        <v>9.1686662918080239E-2</v>
+      </c>
+      <c r="R25" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="S25" s="2">
+        <v>0.10653779584224662</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B26" s="8"/>
+      <c r="C26" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.34049352719813897</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.2089828025596337</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.25285363047005394</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.34637723804815007</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.22206734081123991</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.12873329590613694</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0.29945585947788195</v>
+      </c>
+      <c r="K26" s="2">
+        <v>4.8574192454028511E-2</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0.20004026513292963</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0.14957857610294659</v>
+      </c>
+      <c r="N26" s="2">
+        <v>0.18212350615057971</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0.19309923316520197</v>
+      </c>
+      <c r="R26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S26" s="2">
+        <v>6.2789256474568692E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B27" s="8"/>
+      <c r="C27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="2">
+        <f>(2*D25*D26)/(D25+D26)</f>
+        <v>0.22355353322702062</v>
+      </c>
+      <c r="E27" s="2">
+        <f>(2*E25*E26)/(E25+E26)</f>
+        <v>7.1433685537712371E-2</v>
+      </c>
+      <c r="F27" s="2">
+        <f>(2*F25*F26)/(F25+F26)</f>
+        <v>0.16222225632468984</v>
+      </c>
+      <c r="G27" s="2">
+        <f>(2*G25*G26)/(G25+G26)</f>
+        <v>0.4127404452514491</v>
+      </c>
+      <c r="H27" s="2">
+        <f>(2*H25*H26)/(H25+H26)</f>
+        <v>0.22126370355354699</v>
+      </c>
+      <c r="I27" s="2">
+        <f>(2*I25*I26)/(I25+I26)</f>
+        <v>0.1211690555768651</v>
+      </c>
+      <c r="J27" s="2">
+        <f>(2*J25*J26)/(J25+J26)</f>
+        <v>0.40049183072276184</v>
+      </c>
+      <c r="K27" s="2">
+        <f>(2*K25*K26)/(K25+K26)</f>
+        <v>3.2616967854148485E-2</v>
+      </c>
+      <c r="L27" s="2">
+        <f>(2*L25*L26)/(L25+L26)</f>
+        <v>0.1334742060476953</v>
+      </c>
+      <c r="M27" s="2">
+        <f>(2*M25*M26)/(M25+M26)</f>
+        <v>0.11001274224300948</v>
+      </c>
+      <c r="N27" s="2">
+        <f>(2*N25*N26)/(N25+N26)</f>
+        <v>0.11709951388526367</v>
+      </c>
+      <c r="O27" s="2">
+        <f>(2*O25*O26)/(O25+O26)</f>
+        <v>0.12433638424130491</v>
+      </c>
+      <c r="R27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="S27" s="2">
+        <v>3.1587313482671582E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="S28" s="4"/>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="S29" s="4"/>
+      <c r="W29" s="4"/>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="S30" s="4"/>
+      <c r="W30" s="4"/>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="W31" s="4"/>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="W32" s="4"/>
+    </row>
+    <row r="33" spans="23:23" x14ac:dyDescent="0.3">
+      <c r="W33" s="4"/>
+    </row>
+    <row r="34" spans="23:23" x14ac:dyDescent="0.3">
+      <c r="W34" s="4"/>
+    </row>
+    <row r="35" spans="23:23" x14ac:dyDescent="0.3">
+      <c r="W35" s="4"/>
+    </row>
+    <row r="36" spans="23:23" x14ac:dyDescent="0.3">
+      <c r="W36" s="4"/>
+    </row>
+    <row r="37" spans="23:23" x14ac:dyDescent="0.3">
+      <c r="W37" s="4"/>
+    </row>
+    <row r="38" spans="23:23" x14ac:dyDescent="0.3">
+      <c r="W38" s="4"/>
+    </row>
+    <row r="39" spans="23:23" x14ac:dyDescent="0.3">
+      <c r="W39" s="4"/>
+    </row>
+    <row r="40" spans="23:23" x14ac:dyDescent="0.3">
+      <c r="W40" s="4"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:S27">
+    <sortCondition descending="1" ref="S15"/>
+  </sortState>
   <mergeCells count="2">
     <mergeCell ref="D1:L1"/>
-    <mergeCell ref="W1:AE1"/>
+    <mergeCell ref="Q1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755CB0E3-6498-47B1-B478-E9DCBB7D7A8F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Jedit redundant source files of different branches
</commit_message>
<xml_diff>
--- a/data_files/final_dataset_jss/processed_result.xlsx
+++ b/data_files/final_dataset_jss/processed_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdn769\FindCochangeByClone\data_files\final_dataset_jss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC73231E-909D-4730-B568-304739AAA6CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F475FD1-A885-4B9C-AA02-5BE1C39B904E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-4404" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="36">
   <si>
     <t>ccfinder</t>
   </si>
@@ -106,18 +106,6 @@
     <t>F1 Scores</t>
   </si>
   <si>
-    <t>cw_type1</t>
-  </si>
-  <si>
-    <t>cw_type2blind</t>
-  </si>
-  <si>
-    <t>cw_type3pattern</t>
-  </si>
-  <si>
-    <t>cw_type3token</t>
-  </si>
-  <si>
     <t>Determine Maximum number of cochange with a seed change (Which clone detection tool?)</t>
   </si>
   <si>
@@ -128,13 +116,40 @@
   </si>
   <si>
     <t>Tools</t>
+  </si>
+  <si>
+    <t>clw1</t>
+  </si>
+  <si>
+    <t>clw2Blind</t>
+  </si>
+  <si>
+    <t>clw3Pattern</t>
+  </si>
+  <si>
+    <t>clw3Token</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>token based or line based working good ?</t>
+  </si>
+  <si>
+    <t>types of clone s different</t>
+  </si>
+  <si>
+    <t>Weighted Average</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +161,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -200,6 +222,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -485,7 +520,7 @@
   <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="C25" sqref="C25:P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,28 +541,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="N1" s="11" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="N1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -1107,10 +1142,10 @@
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.3">
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C18" s="6" t="s">
         <v>19</v>
       </c>
@@ -1143,7 +1178,7 @@
       </c>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C19" s="6" t="s">
         <v>21</v>
       </c>
@@ -1176,7 +1211,7 @@
       </c>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C20" s="6" t="s">
         <v>22</v>
       </c>
@@ -1218,26 +1253,142 @@
       </c>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.3">
       <c r="N21" s="4"/>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.3">
       <c r="N22" s="4"/>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.3">
       <c r="N23" s="4"/>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.3">
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="N25" s="4"/>
-    </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="N26" s="4"/>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="N27" s="4"/>
+    <row r="25" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.15028011297791405</v>
+      </c>
+      <c r="F25" s="2">
+        <v>3.766113559099412E-2</v>
+      </c>
+      <c r="G25" s="2">
+        <v>9.9431029220140937E-2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.42253910193057115</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.19855435687747269</v>
+      </c>
+      <c r="J25" s="2">
+        <v>9.9586891490418744E-2</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.45304744081845705</v>
+      </c>
+      <c r="L25" s="2">
+        <v>2.2506997115280855E-2</v>
+      </c>
+      <c r="M25" s="2">
+        <v>9.4156425300352786E-2</v>
+      </c>
+      <c r="N25" s="2">
+        <v>7.9830722933097967E-2</v>
+      </c>
+      <c r="O25" s="2">
+        <v>7.7569641204349588E-2</v>
+      </c>
+      <c r="P25" s="2">
+        <v>8.6474721042650041E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C26" s="7"/>
+      <c r="D26" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.31461118498536067</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.11854657117989277</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.20120668593520663</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.25652997905091446</v>
+      </c>
+      <c r="I26" s="2">
+        <v>4.559407313852238E-2</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0.19444030106848167</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0.14148396358834936</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0.16880169635157233</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0.1861747296935245</v>
+      </c>
+      <c r="N26" s="7"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="7"/>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C27" s="7"/>
+      <c r="D27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" ref="E27:M27" si="3">(2*E25*E26)/(E25+E26)</f>
+        <v>0.20340154625759593</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="3"/>
+        <v>5.7162333195271829E-2</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="3"/>
+        <v>0.13309167053889776</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="3"/>
+        <v>0.31924276926222445</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="3"/>
+        <v>7.4159001299747659E-2</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="3"/>
+        <v>0.13171370304460694</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="3"/>
+        <v>0.2156284668747083</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="3"/>
+        <v>3.9718208555928683E-2</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12506313848408732</v>
+      </c>
+      <c r="N27" s="7"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1254,7 +1405,7 @@
   <dimension ref="A1:AB40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,39 +1426,45 @@
     <col min="16" max="16" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.77734375" style="7" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" style="7" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="6.21875" style="7" bestFit="1" customWidth="1"/>
     <col min="26" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="Q1" s="11" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="Q1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
@@ -1320,16 +1477,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>2</v>
@@ -1352,40 +1509,40 @@
       <c r="O2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" s="8" t="s">
+      <c r="R2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="W2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="X2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Y2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="Z2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AA2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AB2" s="11" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1891,30 +2048,84 @@
       <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
+      <c r="B9" s="7">
+        <v>5122</v>
+      </c>
+      <c r="C9" s="7">
+        <v>323277</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4.8091838763995476E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.5358934740746582E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>6.5015436517153316E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.56931945886931834</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.16138238598659291</v>
+      </c>
+      <c r="I9" s="2">
+        <v>5.8676858741456894E-2</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0.41422278751880653</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>3.346588024082265E-2</v>
+      </c>
+      <c r="M9" s="2">
+        <v>9.5792612105499317E-2</v>
+      </c>
+      <c r="N9" s="2">
+        <v>4.8021271080920802E-2</v>
+      </c>
+      <c r="O9" s="2">
+        <v>2.3913462215803424E-2</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>0.14135096</v>
+      </c>
+      <c r="R9" s="5">
+        <v>6.0063419999999999E-2</v>
+      </c>
+      <c r="S9" s="5">
+        <v>0.11059901</v>
+      </c>
+      <c r="T9" s="5">
+        <v>0.25093423999999998</v>
+      </c>
+      <c r="U9" s="5">
+        <v>0.26085166999999998</v>
+      </c>
+      <c r="V9" s="5">
+        <v>0.14489198</v>
+      </c>
+      <c r="W9" s="5">
+        <v>0.11689541000000001</v>
+      </c>
+      <c r="X9" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>9.5235379999999994E-2</v>
+      </c>
+      <c r="Z9" s="5">
+        <v>0.17213349999999999</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>9.6248840000000002E-2</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>5.194298E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
@@ -1944,10 +2155,10 @@
       <c r="I10" s="2">
         <v>5.0066456251550172E-2</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="5">
         <v>0.50518975920166476</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="5">
         <v>4.7846889952153108E-3</v>
       </c>
       <c r="L10" s="2">
@@ -2000,107 +2211,109 @@
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="D11" s="2">
-        <f>(D3*2909+D4*8052+D5*4582+D6*718+D7*6865+D8*8313+D10*2508)/27082</f>
-        <v>0.16640348285606194</v>
-      </c>
-      <c r="E11" s="2">
-        <f>(E3*2909+E4*8052+E5*4582+E6*718+E7*6865+E8*8313+E10*2508)/27082</f>
-        <v>4.3079471063632781E-2</v>
-      </c>
-      <c r="F11" s="2">
-        <f>(F3*2909+F4*8052+F5*4582+F6*718+F7*6865+F8*8313+F10*2508)/27082</f>
-        <v>0.11941856518794243</v>
-      </c>
-      <c r="G11" s="2">
-        <f>(G3*2909+G4*8052+G5*4582+G6*718+G7*6865+G8*8313+G10*2508)/27082</f>
-        <v>0.5105597567348692</v>
-      </c>
-      <c r="H11" s="2">
-        <f>(H3*2909+H4*8052+H5*4582+H6*718+H7*6865+H8*8313+H10*2508)/27082</f>
-        <v>0.22046586194781462</v>
-      </c>
-      <c r="I11" s="2">
-        <f>(I3*2909+I4*8052+I5*4582+I6*718+I7*6865+I8*8313+I10*2508)/27082</f>
-        <v>0.11444441564834654</v>
-      </c>
-      <c r="J11" s="2">
-        <f>(J3*2909+J4*8052+J5*4582+J6*718+J7*6865+J8*8313+J10*2508)/27082</f>
-        <v>0.6044234097457889</v>
-      </c>
-      <c r="K11" s="2">
-        <f>(K3*2909+K4*8052+K5*4582+K6*718+K7*6865+K8*8313+K10*2508)/27082</f>
-        <v>2.4551496626395251E-2</v>
-      </c>
-      <c r="L11" s="2">
-        <f>(L3*2909+L4*8052+L5*4582+L6*718+L7*6865+L8*8313+L10*2508)/27082</f>
-        <v>0.1001484704098351</v>
-      </c>
-      <c r="M11" s="2">
-        <f>(M3*2909+M4*8052+M5*4582+M6*718+M7*6865+M8*8313+M10*2508)/27082</f>
-        <v>8.6999924158081346E-2</v>
-      </c>
-      <c r="N11" s="2">
-        <f>(N3*2909+N4*8052+N5*4582+N6*718+N7*6865+N8*8313+N10*2508)/27082</f>
-        <v>8.6290875657122651E-2</v>
-      </c>
-      <c r="O11" s="2">
-        <f>(O3*2909+O4*8052+O5*4582+O6*718+O7*6865+O8*8313+O10*2508)/27082</f>
-        <v>9.1686662908834218E-2</v>
-      </c>
-      <c r="Q11" s="2">
-        <f>(Q3*2909+Q4*8052+Q5*4582+Q6*718+Q7*6865+Q8*8313+Q10*2508)/27082</f>
-        <v>0.34049352719813897</v>
-      </c>
-      <c r="R11" s="2">
-        <f t="shared" ref="R11:AB11" si="0">(R3*2909+R4*8052+R5*4582+R6*718+R7*6865+R8*8313+R10*2508)/27082</f>
-        <v>0.12873329590613694</v>
-      </c>
-      <c r="S11" s="2">
+      <c r="C11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="14">
+        <f>(D3*2909+D4*8052+D5*4582+D6*718+D7*6865+D8*8313+D9*5054+D10*2508)/39001</f>
+        <v>0.12178137165255</v>
+      </c>
+      <c r="E11" s="14">
+        <f t="shared" ref="E11:O11" si="0">(E3*2909+E4*8052+E5*4582+E6*718+E7*6865+E8*8313+E9*5054+E10*2508)/39001</f>
+        <v>3.3200233110049389E-2</v>
+      </c>
+      <c r="F11" s="14">
         <f t="shared" si="0"/>
-        <v>0.2089828025596337</v>
-      </c>
-      <c r="T11" s="2">
+        <v>9.1348467951528164E-2</v>
+      </c>
+      <c r="G11" s="14">
         <f t="shared" si="0"/>
-        <v>0.25285363047005394</v>
-      </c>
-      <c r="U11" s="2">
+        <v>0.42830491210531169</v>
+      </c>
+      <c r="H11" s="14">
         <f t="shared" si="0"/>
-        <v>0.34637723804815007</v>
-      </c>
-      <c r="V11" s="2">
+        <v>0.17400279613463646</v>
+      </c>
+      <c r="I11" s="14">
         <f t="shared" si="0"/>
-        <v>0.22206734081123991</v>
-      </c>
-      <c r="W11" s="2">
+        <v>8.7073062451420324E-2</v>
+      </c>
+      <c r="J11" s="14">
         <f t="shared" si="0"/>
-        <v>0.29945585947788195</v>
-      </c>
-      <c r="X11" s="2">
+        <v>0.47338470169625152</v>
+      </c>
+      <c r="K11" s="14">
         <f t="shared" si="0"/>
-        <v>4.8574192454028511E-2</v>
-      </c>
-      <c r="Y11" s="2">
+        <v>1.7048373929797599E-2</v>
+      </c>
+      <c r="L11" s="14">
         <f t="shared" si="0"/>
-        <v>0.20004026513292963</v>
-      </c>
-      <c r="Z11" s="2">
+        <v>7.3879065520788489E-2</v>
+      </c>
+      <c r="M11" s="14">
         <f t="shared" si="0"/>
-        <v>0.14957857610294659</v>
-      </c>
-      <c r="AA11" s="2">
+        <v>7.2825512361999759E-2</v>
+      </c>
+      <c r="N11" s="14">
         <f t="shared" si="0"/>
-        <v>0.18212350615057971</v>
-      </c>
-      <c r="AB11" s="2">
+        <v>6.6142637332098395E-2</v>
+      </c>
+      <c r="O11" s="14">
         <f t="shared" si="0"/>
-        <v>0.19309923316520197</v>
+        <v>6.6765386603823459E-2</v>
+      </c>
+      <c r="Q11" s="14">
+        <f>(Q3*2909+Q4*8052+Q5*4582+Q6*718+Q7*6865+Q8*8313+Q9*5054+Q10*2508)/39001</f>
+        <v>0.25475330005435759</v>
+      </c>
+      <c r="R11" s="14">
+        <f t="shared" ref="R11:AB11" si="1">(R3*2909+R4*8052+R5*4582+R6*718+R7*6865+R8*8313+R9*5054+R10*2508)/39001</f>
+        <v>9.7174832553267879E-2</v>
+      </c>
+      <c r="S11" s="14">
+        <f t="shared" si="1"/>
+        <v>0.15944821044229635</v>
+      </c>
+      <c r="T11" s="14">
+        <f t="shared" si="1"/>
+        <v>0.20809732235968306</v>
+      </c>
+      <c r="U11" s="14">
+        <f t="shared" si="1"/>
+        <v>0.27432457375451913</v>
+      </c>
+      <c r="V11" s="14">
+        <f t="shared" si="1"/>
+        <v>0.17297791827824927</v>
+      </c>
+      <c r="W11" s="14">
+        <f t="shared" si="1"/>
+        <v>0.22308794616855979</v>
+      </c>
+      <c r="X11" s="14">
+        <f t="shared" si="1"/>
+        <v>3.3729552576600604E-2</v>
+      </c>
+      <c r="Y11" s="14">
+        <f t="shared" si="1"/>
+        <v>0.15124766213302224</v>
+      </c>
+      <c r="Z11" s="14">
+        <f t="shared" si="1"/>
+        <v>0.12617239832363272</v>
+      </c>
+      <c r="AA11" s="14">
+        <f t="shared" si="1"/>
+        <v>0.13893773059485653</v>
+      </c>
+      <c r="AB11" s="14">
+        <f t="shared" si="1"/>
+        <v>0.14081775476269839</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="N15" s="9"/>
       <c r="R15" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="S15" s="10" t="s">
         <v>22</v>
@@ -2108,399 +2321,370 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="N16" s="9"/>
-      <c r="R16" s="8" t="s">
+      <c r="R16" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="S16" s="2">
-        <v>0.35280720740855737</v>
-      </c>
-    </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="N17" s="9"/>
-      <c r="R17" s="8" t="s">
+      <c r="S16" s="5">
+        <v>0.30326078467774026</v>
+      </c>
+      <c r="W16" s="13"/>
+    </row>
+    <row r="17" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="S17" s="2">
-        <v>0.31665799211299567</v>
-      </c>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B18" s="7" t="s">
+      <c r="C17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.12178137165255</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3.3200233110049389E-2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>9.1348467951528164E-2</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.42830491210531169</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.17400279613463646</v>
+      </c>
+      <c r="I17" s="2">
+        <v>8.7073062451420324E-2</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.47338470169625152</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1.7048373929797599E-2</v>
+      </c>
+      <c r="L17" s="2">
+        <v>7.3879065520788489E-2</v>
+      </c>
+      <c r="M17" s="2">
+        <v>7.2825512361999759E-2</v>
+      </c>
+      <c r="N17" s="2">
+        <v>6.6142637332098395E-2</v>
+      </c>
+      <c r="O17" s="2">
+        <v>6.6765386603823459E-2</v>
+      </c>
+      <c r="R17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="S17" s="5">
+        <v>0.28010305600998736</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+    </row>
+    <row r="18" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B18" s="8"/>
+      <c r="C18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.25475330005435759</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9.7174832553267879E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.15944821044229635</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.20809732235968306</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.27432457375451913</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.17297791827824927</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.22308794616855979</v>
+      </c>
+      <c r="K18" s="2">
+        <v>3.3729552576600604E-2</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.15124766213302224</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0.12617239832363272</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0.13893773059485653</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.14081775476269839</v>
+      </c>
+      <c r="R18" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="S18" s="5">
+        <v>0.21293923185430416</v>
+      </c>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B19" s="8"/>
+      <c r="C19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="14">
+        <f t="shared" ref="D19:O19" si="2">(2*D17*D18)/(D17+D18)</f>
+        <v>0.16478804553638754</v>
+      </c>
+      <c r="E19" s="14">
+        <f t="shared" si="2"/>
+        <v>4.9491474106405774E-2</v>
+      </c>
+      <c r="F19" s="14">
+        <f t="shared" si="2"/>
+        <v>0.11615265269697667</v>
+      </c>
+      <c r="G19" s="14">
+        <f t="shared" si="2"/>
+        <v>0.28010305600998736</v>
+      </c>
+      <c r="H19" s="14">
+        <f t="shared" si="2"/>
+        <v>0.21293923185430416</v>
+      </c>
+      <c r="I19" s="14">
+        <f t="shared" si="2"/>
+        <v>0.11583664894242998</v>
+      </c>
+      <c r="J19" s="14">
+        <f t="shared" si="2"/>
+        <v>0.30326078467774026</v>
+      </c>
+      <c r="K19" s="14">
+        <f t="shared" si="2"/>
+        <v>2.2648976213638768E-2</v>
+      </c>
+      <c r="L19" s="14">
+        <f t="shared" si="2"/>
+        <v>9.9268852321920079E-2</v>
+      </c>
+      <c r="M19" s="14">
+        <f t="shared" si="2"/>
+        <v>9.234840227419816E-2</v>
+      </c>
+      <c r="N19" s="14">
+        <f t="shared" si="2"/>
+        <v>8.9620552365632156E-2</v>
+      </c>
+      <c r="O19" s="14">
+        <f t="shared" si="2"/>
+        <v>9.0582999905696931E-2</v>
+      </c>
+      <c r="R19" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S19" s="5">
+        <v>0.16478804553638754</v>
+      </c>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="R20" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.15028011297791405</v>
-      </c>
-      <c r="E18" s="2">
-        <v>3.766113559099412E-2</v>
-      </c>
-      <c r="F18" s="2">
-        <v>9.9431029220140937E-2</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0.42253910193057115</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.19855435687747269</v>
-      </c>
-      <c r="I18" s="2">
-        <v>9.9586891490418744E-2</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0.45304744081845705</v>
-      </c>
-      <c r="K18" s="2">
-        <v>2.2506997115280855E-2</v>
-      </c>
-      <c r="L18" s="2">
-        <v>9.4156425300352786E-2</v>
-      </c>
-      <c r="M18" s="2">
-        <v>7.9830722933097967E-2</v>
-      </c>
-      <c r="N18" s="2">
-        <v>7.7569641204349588E-2</v>
-      </c>
-      <c r="O18" s="2">
-        <v>8.6474721042650041E-2</v>
-      </c>
-      <c r="R18" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="S18" s="2">
-        <v>0.25736684309358249</v>
-      </c>
-    </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C19" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.31461118498536067</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.11854657117989277</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0.20120668593520663</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0.25652997905091446</v>
-      </c>
-      <c r="H19" s="2">
-        <v>4.559407313852238E-2</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0.19444030106848167</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0.14148396358834936</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0.16880169635157233</v>
-      </c>
-      <c r="L19" s="2">
-        <v>0.1861747296935245</v>
-      </c>
-      <c r="N19" s="9"/>
-      <c r="R19" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="S19" s="2">
-        <v>0.21545460883405504</v>
-      </c>
-    </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C20" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="2">
-        <f>(2*D18*D19)/(D18+D19)</f>
-        <v>0.20340154625759593</v>
-      </c>
-      <c r="E20" s="2">
-        <f>(2*E18*E19)/(E18+E19)</f>
-        <v>5.7162333195271829E-2</v>
-      </c>
-      <c r="F20" s="2">
-        <f>(2*F18*F19)/(F18+F19)</f>
-        <v>0.13309167053889776</v>
-      </c>
-      <c r="G20" s="2">
-        <f>(2*G18*G19)/(G18+G19)</f>
-        <v>0.31924276926222445</v>
-      </c>
-      <c r="H20" s="2">
-        <f>(2*H18*H19)/(H18+H19)</f>
-        <v>7.4159001299747659E-2</v>
-      </c>
-      <c r="I20" s="2">
-        <f>(2*I18*I19)/(I18+I19)</f>
-        <v>0.13171370304460694</v>
-      </c>
-      <c r="J20" s="2">
-        <f>(2*J18*J19)/(J18+J19)</f>
-        <v>0.2156284668747083</v>
-      </c>
-      <c r="K20" s="2">
-        <f>(2*K18*K19)/(K18+K19)</f>
-        <v>3.9718208555928683E-2</v>
-      </c>
-      <c r="L20" s="2">
-        <f>(2*L18*L19)/(L18+L19)</f>
-        <v>0.12506313848408732</v>
-      </c>
-      <c r="N20" s="9"/>
-      <c r="R20" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="S20" s="2">
-        <v>0.14555626850919298</v>
-      </c>
-    </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="R21" s="8" t="s">
+      <c r="S20" s="5">
+        <v>0.11615265269697667</v>
+      </c>
+      <c r="T20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="R21" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="S21" s="2">
-        <v>0.1443428629641893</v>
-      </c>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="R22" s="8" t="s">
+      <c r="S21" s="5">
+        <v>0.11583664894242998</v>
+      </c>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="D22" s="7">
+        <v>0.16478804553638754</v>
+      </c>
+      <c r="E22" s="7">
+        <v>4.9491474106405774E-2</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0.11615265269697667</v>
+      </c>
+      <c r="G22" s="7">
+        <v>0.28010305600998736</v>
+      </c>
+      <c r="H22" s="7">
+        <v>0.21293923185430416</v>
+      </c>
+      <c r="I22" s="7">
+        <v>0.11583664894242998</v>
+      </c>
+      <c r="J22" s="7">
+        <v>0.30326078467774026</v>
+      </c>
+      <c r="K22" s="7">
+        <v>2.2648976213638768E-2</v>
+      </c>
+      <c r="L22" s="7">
+        <v>9.9268852321920079E-2</v>
+      </c>
+      <c r="M22" s="7">
+        <v>9.234840227419816E-2</v>
+      </c>
+      <c r="N22" s="7">
+        <v>8.9620552365632156E-2</v>
+      </c>
+      <c r="O22" s="7">
+        <v>9.0582999905696931E-2</v>
+      </c>
+      <c r="R22" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S22" s="2">
-        <v>0.13087857231531486</v>
-      </c>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="R23" s="8" t="s">
+      <c r="S22" s="5">
+        <v>9.9268852321920079E-2</v>
+      </c>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="4"/>
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="R23" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S23" s="5">
+        <v>9.234840227419816E-2</v>
+      </c>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="4"/>
+    </row>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="R24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="S23" s="2">
-        <v>0.12166917144513506</v>
-      </c>
-    </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="R24" s="8" t="s">
+      <c r="S24" s="5">
+        <v>9.0582999905696931E-2</v>
+      </c>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="4"/>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="R25" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="S24" s="2">
-        <v>0.11306335716411227</v>
-      </c>
-    </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B25" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.16640348274325442</v>
-      </c>
-      <c r="E25" s="2">
-        <v>4.3079471059581161E-2</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0.11941856530437982</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0.51055975668652631</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0.22046586187181957</v>
-      </c>
-      <c r="I25" s="2">
-        <v>0.11444441562980644</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0.60442340962375296</v>
-      </c>
-      <c r="K25" s="2">
-        <v>2.4551496715014557E-2</v>
-      </c>
-      <c r="L25" s="2">
-        <v>0.10014847038789471</v>
-      </c>
-      <c r="M25" s="2">
-        <v>8.6999924243698012E-2</v>
-      </c>
-      <c r="N25" s="2">
-        <v>8.6290875586467419E-2</v>
-      </c>
-      <c r="O25" s="2">
-        <v>9.1686662918080239E-2</v>
-      </c>
-      <c r="R25" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="S25" s="2">
-        <v>0.10653779584224662</v>
-      </c>
-    </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B26" s="8"/>
-      <c r="C26" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.34049352719813897</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0.2089828025596337</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0.25285363047005394</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0.34637723804815007</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0.22206734081123991</v>
-      </c>
-      <c r="I26" s="2">
-        <v>0.12873329590613694</v>
-      </c>
-      <c r="J26" s="2">
-        <v>0.29945585947788195</v>
-      </c>
-      <c r="K26" s="2">
-        <v>4.8574192454028511E-2</v>
-      </c>
-      <c r="L26" s="2">
-        <v>0.20004026513292963</v>
-      </c>
-      <c r="M26" s="2">
-        <v>0.14957857610294659</v>
-      </c>
-      <c r="N26" s="2">
-        <v>0.18212350615057971</v>
-      </c>
-      <c r="O26" s="2">
-        <v>0.19309923316520197</v>
-      </c>
-      <c r="R26" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="S26" s="2">
-        <v>6.2789256474568692E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B27" s="8"/>
-      <c r="C27" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="2">
-        <f>(2*D25*D26)/(D25+D26)</f>
-        <v>0.22355353322702062</v>
-      </c>
-      <c r="E27" s="2">
-        <f>(2*E25*E26)/(E25+E26)</f>
-        <v>7.1433685537712371E-2</v>
-      </c>
-      <c r="F27" s="2">
-        <f>(2*F25*F26)/(F25+F26)</f>
-        <v>0.16222225632468984</v>
-      </c>
-      <c r="G27" s="2">
-        <f>(2*G25*G26)/(G25+G26)</f>
-        <v>0.4127404452514491</v>
-      </c>
-      <c r="H27" s="2">
-        <f>(2*H25*H26)/(H25+H26)</f>
-        <v>0.22126370355354699</v>
-      </c>
-      <c r="I27" s="2">
-        <f>(2*I25*I26)/(I25+I26)</f>
-        <v>0.1211690555768651</v>
-      </c>
-      <c r="J27" s="2">
-        <f>(2*J25*J26)/(J25+J26)</f>
-        <v>0.40049183072276184</v>
-      </c>
-      <c r="K27" s="2">
-        <f>(2*K25*K26)/(K25+K26)</f>
-        <v>3.2616967854148485E-2</v>
-      </c>
-      <c r="L27" s="2">
-        <f>(2*L25*L26)/(L25+L26)</f>
-        <v>0.1334742060476953</v>
-      </c>
-      <c r="M27" s="2">
-        <f>(2*M25*M26)/(M25+M26)</f>
-        <v>0.11001274224300948</v>
-      </c>
-      <c r="N27" s="2">
-        <f>(2*N25*N26)/(N25+N26)</f>
-        <v>0.11709951388526367</v>
-      </c>
-      <c r="O27" s="2">
-        <f>(2*O25*O26)/(O25+O26)</f>
-        <v>0.12433638424130491</v>
-      </c>
-      <c r="R27" s="8" t="s">
+      <c r="S25" s="5">
+        <v>8.9620552365632156E-2</v>
+      </c>
+      <c r="W25" s="13"/>
+      <c r="X25" s="13"/>
+      <c r="Y25" s="4"/>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="R26" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S26" s="5">
+        <v>4.9491474106405774E-2</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="W26" s="13"/>
+      <c r="X26" s="13"/>
+      <c r="Y26" s="4"/>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="R27" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="S27" s="2">
-        <v>3.1587313482671582E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="S27" s="5">
+        <v>2.2648976213638768E-2</v>
+      </c>
+      <c r="Y27" s="4"/>
+    </row>
+    <row r="28" spans="2:25" x14ac:dyDescent="0.3">
       <c r="S28" s="4"/>
-    </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y28" s="4"/>
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.3">
       <c r="S29" s="4"/>
       <c r="W29" s="4"/>
-    </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y29" s="4"/>
+    </row>
+    <row r="30" spans="2:25" x14ac:dyDescent="0.3">
       <c r="S30" s="4"/>
       <c r="W30" s="4"/>
-    </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y30" s="4"/>
+    </row>
+    <row r="31" spans="2:25" x14ac:dyDescent="0.3">
       <c r="W31" s="4"/>
-    </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y31" s="4"/>
+    </row>
+    <row r="32" spans="2:25" x14ac:dyDescent="0.3">
       <c r="W32" s="4"/>
-    </row>
-    <row r="33" spans="23:23" x14ac:dyDescent="0.3">
+      <c r="Y32" s="4"/>
+    </row>
+    <row r="33" spans="9:25" x14ac:dyDescent="0.3">
       <c r="W33" s="4"/>
-    </row>
-    <row r="34" spans="23:23" x14ac:dyDescent="0.3">
+      <c r="Y33" s="4"/>
+    </row>
+    <row r="34" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="K34" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="W34" s="4"/>
     </row>
-    <row r="35" spans="23:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I35" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="W35" s="4"/>
     </row>
-    <row r="36" spans="23:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="9:25" x14ac:dyDescent="0.3">
       <c r="W36" s="4"/>
     </row>
-    <row r="37" spans="23:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="9:25" x14ac:dyDescent="0.3">
       <c r="W37" s="4"/>
     </row>
-    <row r="38" spans="23:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="9:25" x14ac:dyDescent="0.3">
       <c r="W38" s="4"/>
     </row>
-    <row r="39" spans="23:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="9:25" x14ac:dyDescent="0.3">
       <c r="W39" s="4"/>
     </row>
-    <row r="40" spans="23:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="9:25" x14ac:dyDescent="0.3">
       <c r="W40" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:S27">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:T27">
     <sortCondition descending="1" ref="S15"/>
   </sortState>
   <mergeCells count="2">
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="Q1:Y1"/>
+    <mergeCell ref="Q1:AB1"/>
+    <mergeCell ref="D1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2516,7 +2700,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started Updating the paper for JSS clone special issue
</commit_message>
<xml_diff>
--- a/data_files/final_dataset_jss/processed_result.xlsx
+++ b/data_files/final_dataset_jss/processed_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdn769\FindCochangeByClone\data_files\final_dataset_jss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F475FD1-A885-4B9C-AA02-5BE1C39B904E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB72CB9-7F24-40E1-8E1A-53001B7F723C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-4404" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
   <si>
     <t>ccfinder</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Before</t>
   </si>
   <si>
-    <t>After</t>
-  </si>
-  <si>
     <t>Tools</t>
   </si>
   <si>
@@ -143,13 +140,112 @@
   </si>
   <si>
     <t>Weighted Average</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>Clone Detectors</t>
+  </si>
+  <si>
+    <t>CCFinder</t>
+  </si>
+  <si>
+    <t>ConQAT</t>
+  </si>
+  <si>
+    <t>Deckard</t>
+  </si>
+  <si>
+    <t>Duplo</t>
+  </si>
+  <si>
+    <t>iClones</t>
+  </si>
+  <si>
+    <t>Nicad</t>
+  </si>
+  <si>
+    <t>SimCAD</t>
+  </si>
+  <si>
+    <t>Simian</t>
+  </si>
+  <si>
+    <t>CLW(3Pattern)</t>
+  </si>
+  <si>
+    <t>CLW(3Token)</t>
+  </si>
+  <si>
+    <t>CLW(2Blind)</t>
+  </si>
+  <si>
+    <t>CLW(Type1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +268,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -193,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -234,7 +343,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -541,28 +663,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="N1" s="15" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="N1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -1402,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543A9E21-8676-454E-8886-AC1E8BC656F1}">
-  <dimension ref="A1:AB40"/>
+  <dimension ref="A1:BP53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1414,7 +1536,7 @@
     <col min="2" max="2" width="17.21875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" style="7" bestFit="1" customWidth="1"/>
@@ -1437,34 +1559,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="Q1" s="16" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="Q1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
@@ -1474,76 +1596,76 @@
         <v>10</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>27</v>
+        <v>56</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="V2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB2" s="11" t="s">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="W2" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="X2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y2" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z2" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA2" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB2" s="16" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
@@ -2212,7 +2334,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C11" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="14">
         <f>(D3*2909+D4*8052+D5*4582+D6*718+D7*6865+D8*8313+D9*5054+D10*2508)/39001</f>
@@ -2312,14 +2434,42 @@
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="C15" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="R15" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S15" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="C16" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.47338470169625152</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.22308794616855979</v>
+      </c>
+      <c r="F16" s="14">
+        <f>(2*D16*E16)/(D16+E16)</f>
+        <v>0.30326078467774026</v>
+      </c>
+      <c r="G16" s="21">
+        <v>1</v>
+      </c>
       <c r="N16" s="9"/>
       <c r="R16" s="12" t="s">
         <v>3</v>
@@ -2330,103 +2480,71 @@
       <c r="W16" s="13"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>19</v>
+      <c r="B17" s="8"/>
+      <c r="C17" s="16" t="s">
+        <v>64</v>
       </c>
       <c r="D17" s="2">
-        <v>0.12178137165255</v>
+        <v>0.42830491210531169</v>
       </c>
       <c r="E17" s="2">
-        <v>3.3200233110049389E-2</v>
-      </c>
-      <c r="F17" s="2">
-        <v>9.1348467951528164E-2</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0.42830491210531169</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0.17400279613463646</v>
-      </c>
-      <c r="I17" s="2">
-        <v>8.7073062451420324E-2</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0.47338470169625152</v>
-      </c>
-      <c r="K17" s="2">
-        <v>1.7048373929797599E-2</v>
-      </c>
-      <c r="L17" s="2">
-        <v>7.3879065520788489E-2</v>
-      </c>
-      <c r="M17" s="2">
-        <v>7.2825512361999759E-2</v>
-      </c>
-      <c r="N17" s="2">
-        <v>6.6142637332098395E-2</v>
-      </c>
-      <c r="O17" s="2">
-        <v>6.6765386603823459E-2</v>
-      </c>
+        <v>0.20809732235968306</v>
+      </c>
+      <c r="F17" s="14">
+        <f>(2*D17*E17)/(D17+E17)</f>
+        <v>0.28010305600998736</v>
+      </c>
+      <c r="G17" s="21">
+        <v>2</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
       <c r="R17" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S17" s="5">
         <v>0.28010305600998736</v>
       </c>
       <c r="T17" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W17" s="13"/>
       <c r="X17" s="13"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B18" s="8"/>
-      <c r="C18" s="10" t="s">
-        <v>21</v>
+      <c r="C18" s="16" t="s">
+        <v>65</v>
       </c>
       <c r="D18" s="2">
-        <v>0.25475330005435759</v>
+        <v>0.17400279613463646</v>
       </c>
       <c r="E18" s="2">
-        <v>9.7174832553267879E-2</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0.15944821044229635</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0.20809732235968306</v>
-      </c>
-      <c r="H18" s="2">
         <v>0.27432457375451913</v>
       </c>
-      <c r="I18" s="2">
-        <v>0.17297791827824927</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0.22308794616855979</v>
-      </c>
-      <c r="K18" s="2">
-        <v>3.3729552576600604E-2</v>
-      </c>
-      <c r="L18" s="2">
-        <v>0.15124766213302224</v>
-      </c>
-      <c r="M18" s="2">
-        <v>0.12617239832363272</v>
-      </c>
-      <c r="N18" s="2">
-        <v>0.13893773059485653</v>
-      </c>
-      <c r="O18" s="2">
-        <v>0.14081775476269839</v>
-      </c>
+      <c r="F18" s="14">
+        <f>(2*D18*E18)/(D18+E18)</f>
+        <v>0.21293923185430416</v>
+      </c>
+      <c r="G18" s="21">
+        <v>3</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
       <c r="R18" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S18" s="5">
         <v>0.21293923185430416</v>
@@ -2436,57 +2554,30 @@
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B19" s="8"/>
-      <c r="C19" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="14">
-        <f t="shared" ref="D19:O19" si="2">(2*D17*D18)/(D17+D18)</f>
+      <c r="C19" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.12178137165255</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.25475330005435759</v>
+      </c>
+      <c r="F19" s="14">
+        <f>(2*D19*E19)/(D19+E19)</f>
         <v>0.16478804553638754</v>
       </c>
-      <c r="E19" s="14">
-        <f t="shared" si="2"/>
-        <v>4.9491474106405774E-2</v>
-      </c>
-      <c r="F19" s="14">
-        <f t="shared" si="2"/>
-        <v>0.11615265269697667</v>
-      </c>
-      <c r="G19" s="14">
-        <f t="shared" si="2"/>
-        <v>0.28010305600998736</v>
-      </c>
-      <c r="H19" s="14">
-        <f t="shared" si="2"/>
-        <v>0.21293923185430416</v>
-      </c>
-      <c r="I19" s="14">
-        <f t="shared" si="2"/>
-        <v>0.11583664894242998</v>
-      </c>
-      <c r="J19" s="14">
-        <f t="shared" si="2"/>
-        <v>0.30326078467774026</v>
-      </c>
-      <c r="K19" s="14">
-        <f t="shared" si="2"/>
-        <v>2.2648976213638768E-2</v>
-      </c>
-      <c r="L19" s="14">
-        <f t="shared" si="2"/>
-        <v>9.9268852321920079E-2</v>
-      </c>
-      <c r="M19" s="14">
-        <f t="shared" si="2"/>
-        <v>9.234840227419816E-2</v>
-      </c>
-      <c r="N19" s="14">
-        <f t="shared" si="2"/>
-        <v>8.9620552365632156E-2</v>
-      </c>
-      <c r="O19" s="14">
-        <f t="shared" si="2"/>
-        <v>9.0582999905696931E-2</v>
-      </c>
+      <c r="G19" s="21">
+        <v>4</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
       <c r="R19" s="12" t="s">
         <v>0</v>
       </c>
@@ -2497,19 +2588,51 @@
       <c r="X19" s="13"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="C20" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="2">
+        <v>9.1348467951528164E-2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.15944821044229635</v>
+      </c>
+      <c r="F20" s="14">
+        <f>(2*D20*E20)/(D20+E20)</f>
+        <v>0.11615265269697667</v>
+      </c>
+      <c r="G20" s="21">
+        <v>5</v>
+      </c>
       <c r="R20" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S20" s="5">
         <v>0.11615265269697667</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W20" s="13"/>
       <c r="X20" s="13"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="C21" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="2">
+        <v>8.7073062451420324E-2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.17297791827824927</v>
+      </c>
+      <c r="F21" s="14">
+        <f>(2*D21*E21)/(D21+E21)</f>
+        <v>0.11583664894242998</v>
+      </c>
+      <c r="G21" s="21">
+        <v>6</v>
+      </c>
       <c r="R21" s="12" t="s">
         <v>2</v>
       </c>
@@ -2520,41 +2643,21 @@
       <c r="X21" s="13"/>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="D22" s="7">
-        <v>0.16478804553638754</v>
-      </c>
-      <c r="E22" s="7">
-        <v>4.9491474106405774E-2</v>
-      </c>
-      <c r="F22" s="7">
-        <v>0.11615265269697667</v>
-      </c>
-      <c r="G22" s="7">
-        <v>0.28010305600998736</v>
-      </c>
-      <c r="H22" s="7">
-        <v>0.21293923185430416</v>
-      </c>
-      <c r="I22" s="7">
-        <v>0.11583664894242998</v>
-      </c>
-      <c r="J22" s="7">
-        <v>0.30326078467774026</v>
-      </c>
-      <c r="K22" s="7">
-        <v>2.2648976213638768E-2</v>
-      </c>
-      <c r="L22" s="7">
+      <c r="C22" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="2">
+        <v>7.3879065520788489E-2</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.15124766213302224</v>
+      </c>
+      <c r="F22" s="14">
+        <f>(2*D22*E22)/(D22+E22)</f>
         <v>9.9268852321920079E-2</v>
       </c>
-      <c r="M22" s="7">
-        <v>9.234840227419816E-2</v>
-      </c>
-      <c r="N22" s="7">
-        <v>8.9620552365632156E-2</v>
-      </c>
-      <c r="O22" s="7">
-        <v>9.0582999905696931E-2</v>
+      <c r="G22" s="21">
+        <v>7</v>
       </c>
       <c r="R22" s="12" t="s">
         <v>5</v>
@@ -2567,6 +2670,22 @@
       <c r="Y22" s="4"/>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="C23" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="2">
+        <v>7.2825512361999759E-2</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.12617239832363272</v>
+      </c>
+      <c r="F23" s="14">
+        <f>(2*D23*E23)/(D23+E23)</f>
+        <v>9.234840227419816E-2</v>
+      </c>
+      <c r="G23" s="21">
+        <v>8</v>
+      </c>
       <c r="R23" s="12" t="s">
         <v>6</v>
       </c>
@@ -2578,6 +2697,22 @@
       <c r="Y23" s="4"/>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="C24" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="2">
+        <v>6.6765386603823459E-2</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.14081775476269839</v>
+      </c>
+      <c r="F24" s="14">
+        <f>(2*D24*E24)/(D24+E24)</f>
+        <v>9.0582999905696931E-2</v>
+      </c>
+      <c r="G24" s="21">
+        <v>9</v>
+      </c>
       <c r="R24" s="12" t="s">
         <v>8</v>
       </c>
@@ -2589,6 +2724,22 @@
       <c r="Y24" s="4"/>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="C25" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="2">
+        <v>6.6142637332098395E-2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.13893773059485653</v>
+      </c>
+      <c r="F25" s="14">
+        <f>(2*D25*E25)/(D25+E25)</f>
+        <v>8.9620552365632156E-2</v>
+      </c>
+      <c r="G25" s="21">
+        <v>10</v>
+      </c>
       <c r="R25" s="12" t="s">
         <v>7</v>
       </c>
@@ -2600,20 +2751,52 @@
       <c r="Y25" s="4"/>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="C26" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="2">
+        <v>3.3200233110049389E-2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>9.7174832553267879E-2</v>
+      </c>
+      <c r="F26" s="14">
+        <f>(2*D26*E26)/(D26+E26)</f>
+        <v>4.9491474106405774E-2</v>
+      </c>
+      <c r="G26" s="21">
+        <v>11</v>
+      </c>
       <c r="R26" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S26" s="5">
         <v>4.9491474106405774E-2</v>
       </c>
       <c r="T26" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W26" s="13"/>
       <c r="X26" s="13"/>
       <c r="Y26" s="4"/>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="C27" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1.7048373929797599E-2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>3.3729552576600604E-2</v>
+      </c>
+      <c r="F27" s="14">
+        <f>(2*D27*E27)/(D27+E27)</f>
+        <v>2.2648976213638768E-2</v>
+      </c>
+      <c r="G27" s="21">
+        <v>12</v>
+      </c>
       <c r="R27" s="12" t="s">
         <v>4</v>
       </c>
@@ -2650,13 +2833,13 @@
     </row>
     <row r="34" spans="9:25" x14ac:dyDescent="0.3">
       <c r="K34" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W34" s="4"/>
     </row>
     <row r="35" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I35" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W35" s="4"/>
     </row>
@@ -2675,14 +2858,96 @@
     <row r="40" spans="9:25" x14ac:dyDescent="0.3">
       <c r="W40" s="4"/>
     </row>
+    <row r="53" spans="30:68" x14ac:dyDescent="0.3">
+      <c r="AD53" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE53" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF53" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG53" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH53" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI53" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ53" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK53" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL53" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM53" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN53" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO53" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP53" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ53" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR53" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AS53" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="AT53" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU53" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV53" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AW53" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX53" s="15"/>
+      <c r="AY53" s="15"/>
+      <c r="AZ53" s="15"/>
+      <c r="BA53" s="15"/>
+      <c r="BB53" s="15"/>
+      <c r="BC53" s="15"/>
+      <c r="BD53" s="15"/>
+      <c r="BE53" s="15"/>
+      <c r="BF53" s="15"/>
+      <c r="BG53" s="15"/>
+      <c r="BH53" s="15"/>
+      <c r="BI53" s="15"/>
+      <c r="BJ53" s="15"/>
+      <c r="BK53" s="15"/>
+      <c r="BL53" s="15"/>
+      <c r="BM53" s="15"/>
+      <c r="BN53" s="15"/>
+      <c r="BO53" s="15"/>
+      <c r="BP53" s="15"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:T27">
-    <sortCondition descending="1" ref="S15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C16:F27">
+    <sortCondition descending="1" ref="F15"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="Q1:AB1"/>
     <mergeCell ref="D1:O1"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Did some updates in the images
</commit_message>
<xml_diff>
--- a/data_files/final_dataset_jss/processed_result.xlsx
+++ b/data_files/final_dataset_jss/processed_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdn769\FindCochangeByClone\data_files\final_dataset_jss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C369B29-D0AF-4343-A621-4CBBAE464ED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3FC79E-784D-4866-BEB9-D203C6EB9CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-4404" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-4404" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cw_separate_types" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="167">
   <si>
     <t>ccfinder</t>
   </si>
@@ -521,12 +521,45 @@
   <si>
     <t xml:space="preserve"> % of Line Coverage by Clone Fragments</t>
   </si>
+  <si>
+    <t>Ranking based on sum of ranks in individual systems</t>
+  </si>
+  <si>
+    <t>Final Rank</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>Sum of Ranks</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,6 +645,12 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -665,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -784,9 +823,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -795,6 +831,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3591,11 +3642,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:pattFill prst="smGrid">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -3710,11 +3768,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:pattFill prst="zigZag">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -3829,11 +3894,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
+            <a:pattFill prst="openDmnd">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -3948,11 +4020,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
+            <a:pattFill prst="wdDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -4067,11 +4146,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
+            <a:pattFill prst="dkHorz">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -4186,11 +4272,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
+            <a:pattFill prst="shingle">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -4305,13 +4398,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:pattFill prst="lgCheck">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -4426,13 +4524,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:pattFill prst="pct20">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -4552,6 +4655,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4819,11 +4936,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:pattFill prst="smGrid">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -4938,11 +5062,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:pattFill prst="zigZag">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -5057,11 +5188,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
+            <a:pattFill prst="pct30">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -5176,11 +5314,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
+            <a:pattFill prst="wdDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -5295,11 +5440,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
+            <a:pattFill prst="dkHorz">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -5414,11 +5566,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
+            <a:pattFill prst="lgConfetti">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -5533,13 +5692,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:pattFill prst="solidDmnd">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -5654,13 +5818,18 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:pattFill prst="pct20">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -5780,6 +5949,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5993,10 +6176,14 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="tx1">
+                <a:alpha val="60000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -6169,10 +6356,14 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="tx1">
+                <a:alpha val="20000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -6350,6 +6541,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -10742,48 +10947,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41">
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="Q1" s="42" t="s">
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="Q1" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="42"/>
-      <c r="AD1" s="42" t="s">
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AD1" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="AE1" s="42"/>
-      <c r="AF1" s="42"/>
-      <c r="AG1" s="42"/>
-      <c r="AH1" s="42"/>
-      <c r="AI1" s="42"/>
-      <c r="AJ1" s="42"/>
-      <c r="AK1" s="42"/>
-      <c r="AL1" s="42"/>
-      <c r="AM1" s="42"/>
-      <c r="AN1" s="42"/>
-      <c r="AO1" s="42"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="51"/>
+      <c r="AN1" s="51"/>
+      <c r="AO1" s="51"/>
     </row>
     <row r="2" spans="1:41">
       <c r="A2" s="5" t="s">
@@ -12336,13 +12541,13 @@
       <c r="Y22" s="2"/>
     </row>
     <row r="23" spans="1:25">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
       <c r="R23" s="9" t="s">
         <v>5</v>
       </c>
@@ -12354,13 +12559,13 @@
       <c r="Y23" s="2"/>
     </row>
     <row r="24" spans="1:25">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
       <c r="R24" s="9" t="s">
         <v>7</v>
       </c>
@@ -12372,13 +12577,13 @@
       <c r="Y24" s="2"/>
     </row>
     <row r="25" spans="1:25">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
       <c r="R25" s="9" t="s">
         <v>6</v>
       </c>
@@ -12564,8 +12769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7456461C-E2A3-44D7-A21C-7E2601ED2580}">
   <dimension ref="A1:AN29"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="X37" sqref="X37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12575,29 +12780,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
       <c r="J1" s="40"/>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="18" t="s">
@@ -13465,10 +13670,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB317F8-1811-40BD-9FF4-3B66CC20E864}">
-  <dimension ref="A1:AB47"/>
+  <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AS13" sqref="AS13"/>
+    <sheetView topLeftCell="V16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Y43" sqref="Y43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14038,13 +14243,13 @@
       </c>
     </row>
     <row r="13" spans="1:28">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
     </row>
     <row r="14" spans="1:28">
       <c r="A14" s="16" t="s">
@@ -15016,18 +15221,18 @@
       </c>
     </row>
     <row r="33" spans="1:17">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="52"/>
+      <c r="J33" s="52"/>
     </row>
     <row r="34" spans="1:17">
       <c r="C34" s="18" t="s">
@@ -15071,31 +15276,31 @@
       </c>
     </row>
     <row r="35" spans="1:17">
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="C35" s="46">
+      <c r="C35" s="45">
         <v>2113</v>
       </c>
-      <c r="D35" s="46">
+      <c r="D35" s="45">
         <v>301</v>
       </c>
-      <c r="E35" s="46">
+      <c r="E35" s="45">
         <v>1700</v>
       </c>
-      <c r="F35" s="46">
+      <c r="F35" s="45">
         <v>774</v>
       </c>
-      <c r="G35" s="46">
+      <c r="G35" s="45">
         <v>1001</v>
       </c>
-      <c r="H35" s="46">
+      <c r="H35" s="45">
         <v>1540</v>
       </c>
-      <c r="I35" s="46">
+      <c r="I35" s="45">
         <v>215</v>
       </c>
-      <c r="J35" s="46">
+      <c r="J35" s="45">
         <v>317</v>
       </c>
       <c r="K35" s="41" t="s">
@@ -15126,31 +15331,31 @@
       <c r="B36" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="47">
+      <c r="C36" s="46">
         <v>3122.9715999999999</v>
       </c>
-      <c r="D36" s="47">
+      <c r="D36" s="46">
         <v>13347.5681</v>
       </c>
-      <c r="E36" s="47">
+      <c r="E36" s="46">
         <v>1217.4851000000001</v>
       </c>
-      <c r="F36" s="47">
+      <c r="F36" s="46">
         <v>1110.6234999999999</v>
       </c>
-      <c r="G36" s="47">
+      <c r="G36" s="46">
         <v>6512.991</v>
       </c>
-      <c r="H36" s="47">
+      <c r="H36" s="46">
         <v>4310.8869000000004</v>
       </c>
-      <c r="I36" s="47">
+      <c r="I36" s="46">
         <v>1786.1611</v>
       </c>
-      <c r="J36" s="47">
+      <c r="J36" s="46">
         <v>570.30029999999999</v>
       </c>
-      <c r="K36" s="48">
+      <c r="K36" s="47">
         <f>(C36*2113+D36*301+E36*1700+F36*774+G36*1001+H36*1540+I36*215+J36*317)/7961</f>
         <v>3425.3088677929909</v>
       </c>
@@ -15179,31 +15384,31 @@
       <c r="B37" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="47">
+      <c r="C37" s="46">
         <v>1066.8404</v>
       </c>
-      <c r="D37" s="47">
+      <c r="D37" s="46">
         <v>693.83720000000005</v>
       </c>
-      <c r="E37" s="47">
+      <c r="E37" s="46">
         <v>1327.2557999999999</v>
       </c>
-      <c r="F37" s="47">
+      <c r="F37" s="46">
         <v>141.489</v>
       </c>
-      <c r="G37" s="47">
+      <c r="G37" s="46">
         <v>2500.1028999999999</v>
       </c>
-      <c r="H37" s="47">
+      <c r="H37" s="46">
         <v>1040.9181000000001</v>
       </c>
-      <c r="I37" s="47">
+      <c r="I37" s="46">
         <v>5831.0568999999996</v>
       </c>
-      <c r="J37" s="47">
+      <c r="J37" s="46">
         <v>174.5942</v>
       </c>
-      <c r="K37" s="48">
+      <c r="K37" s="47">
         <f t="shared" ref="K37:K47" si="3">(C37*2113+D37*301+E37*1700+F37*774+G37*1001+H37*1540+I37*215+J37*317)/7961</f>
         <v>1286.7185755809573</v>
       </c>
@@ -15232,31 +15437,31 @@
       <c r="B38" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="47">
+      <c r="C38" s="46">
         <v>1771.6856</v>
       </c>
-      <c r="D38" s="47">
+      <c r="D38" s="46">
         <v>836.30560000000003</v>
       </c>
-      <c r="E38" s="47">
+      <c r="E38" s="46">
         <v>2814.6275000000001</v>
       </c>
-      <c r="F38" s="47">
+      <c r="F38" s="46">
         <v>311.97539999999998</v>
       </c>
-      <c r="G38" s="47">
+      <c r="G38" s="46">
         <v>5371.1129000000001</v>
       </c>
-      <c r="H38" s="47">
+      <c r="H38" s="46">
         <v>2463.2248</v>
       </c>
-      <c r="I38" s="47">
+      <c r="I38" s="46">
         <v>6228.8577999999998</v>
       </c>
-      <c r="J38" s="47">
+      <c r="J38" s="46">
         <v>299.07990000000001</v>
       </c>
-      <c r="K38" s="48">
+      <c r="K38" s="47">
         <f t="shared" si="3"/>
         <v>2465.2051662102749</v>
       </c>
@@ -15285,31 +15490,31 @@
       <c r="B39" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="47">
+      <c r="C39" s="46">
         <v>3555.6889000000001</v>
       </c>
-      <c r="D39" s="47">
+      <c r="D39" s="46">
         <v>1128.3223</v>
       </c>
-      <c r="E39" s="47">
+      <c r="E39" s="46">
         <v>5685.2114000000001</v>
       </c>
-      <c r="F39" s="47">
+      <c r="F39" s="46">
         <v>747.21600000000001</v>
       </c>
-      <c r="G39" s="47">
+      <c r="G39" s="46">
         <v>8510.2886999999992</v>
       </c>
-      <c r="H39" s="47">
+      <c r="H39" s="46">
         <v>4036.4828000000002</v>
       </c>
-      <c r="I39" s="47">
+      <c r="I39" s="46">
         <v>8541.1280000000006</v>
       </c>
-      <c r="J39" s="47">
+      <c r="J39" s="46">
         <v>552.56550000000004</v>
       </c>
-      <c r="K39" s="48">
+      <c r="K39" s="47">
         <f t="shared" si="3"/>
         <v>4376.6472184650174</v>
       </c>
@@ -15338,31 +15543,31 @@
       <c r="B40" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="47">
+      <c r="C40" s="46">
         <v>2360.7154</v>
       </c>
-      <c r="D40" s="47">
+      <c r="D40" s="46">
         <v>1079.1429000000001</v>
       </c>
-      <c r="E40" s="47">
+      <c r="E40" s="46">
         <v>2148.2575000000002</v>
       </c>
-      <c r="F40" s="47">
+      <c r="F40" s="46">
         <v>425.41910000000001</v>
       </c>
-      <c r="G40" s="47">
+      <c r="G40" s="46">
         <v>4065.7013000000002</v>
       </c>
-      <c r="H40" s="47">
+      <c r="H40" s="46">
         <v>1888.9641999999999</v>
       </c>
-      <c r="I40" s="47">
+      <c r="I40" s="46">
         <v>6530.2275</v>
       </c>
-      <c r="J40" s="47">
+      <c r="J40" s="46">
         <v>367.69970000000001</v>
       </c>
-      <c r="K40" s="48">
+      <c r="K40" s="47">
         <f t="shared" si="3"/>
         <v>2235.1033002386639</v>
       </c>
@@ -15391,31 +15596,31 @@
       <c r="B41" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="47">
+      <c r="C41" s="46">
         <v>1647.1775</v>
       </c>
-      <c r="D41" s="47">
+      <c r="D41" s="46">
         <v>1186.9069999999999</v>
       </c>
-      <c r="E41" s="47">
+      <c r="E41" s="46">
         <v>622.67690000000005</v>
       </c>
-      <c r="F41" s="47">
+      <c r="F41" s="46">
         <v>430.54590000000002</v>
       </c>
-      <c r="G41" s="47">
+      <c r="G41" s="46">
         <v>2624.6464000000001</v>
       </c>
-      <c r="H41" s="47">
+      <c r="H41" s="46">
         <v>1285.5345</v>
       </c>
-      <c r="I41" s="47">
+      <c r="I41" s="46">
         <v>4040.6635000000001</v>
       </c>
-      <c r="J41" s="47">
+      <c r="J41" s="46">
         <v>251</v>
       </c>
-      <c r="K41" s="48">
+      <c r="K41" s="47">
         <f t="shared" si="3"/>
         <v>1354.7094774525817</v>
       </c>
@@ -15444,31 +15649,31 @@
       <c r="B42" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="47">
+      <c r="C42" s="46">
         <v>3257.7557999999999</v>
       </c>
-      <c r="D42" s="47">
+      <c r="D42" s="46">
         <v>5364.4291000000003</v>
       </c>
-      <c r="E42" s="47">
+      <c r="E42" s="46">
         <v>4118.5020999999997</v>
       </c>
-      <c r="F42" s="47">
+      <c r="F42" s="46">
         <v>356.33640000000003</v>
       </c>
-      <c r="G42" s="47">
+      <c r="G42" s="46">
         <v>8516.0689000000002</v>
       </c>
-      <c r="H42" s="47">
+      <c r="H42" s="46">
         <v>6806.1857</v>
       </c>
-      <c r="I42" s="47">
+      <c r="I42" s="46">
         <v>14346.663500000001</v>
       </c>
-      <c r="J42" s="47">
+      <c r="J42" s="46">
         <v>1501.2109</v>
       </c>
-      <c r="K42" s="48">
+      <c r="K42" s="47">
         <f t="shared" si="3"/>
         <v>4816.2437586735341</v>
       </c>
@@ -15497,31 +15702,31 @@
       <c r="B43" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="47">
+      <c r="C43" s="46">
         <v>381.05349999999999</v>
       </c>
-      <c r="D43" s="47">
+      <c r="D43" s="46">
         <v>104.7244</v>
       </c>
-      <c r="E43" s="47">
+      <c r="E43" s="46">
         <v>126.44499999999999</v>
       </c>
-      <c r="F43" s="47">
+      <c r="F43" s="46">
         <v>17.697299999999998</v>
       </c>
-      <c r="G43" s="47">
+      <c r="G43" s="46">
         <v>215.58439999999999</v>
       </c>
-      <c r="H43" s="47">
+      <c r="H43" s="46">
         <v>209.01820000000001</v>
       </c>
-      <c r="I43" s="47">
+      <c r="I43" s="46">
         <v>2.7618999999999998</v>
       </c>
-      <c r="J43" s="47">
+      <c r="J43" s="46">
         <v>40.594200000000001</v>
       </c>
-      <c r="K43" s="48">
+      <c r="K43" s="47">
         <f t="shared" si="3"/>
         <v>203.05143605074741</v>
       </c>
@@ -15550,31 +15755,31 @@
       <c r="B44" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="47">
+      <c r="C44" s="46">
         <v>769.52059999999994</v>
       </c>
-      <c r="D44" s="47">
+      <c r="D44" s="46">
         <v>661.63599999999997</v>
       </c>
-      <c r="E44" s="47">
+      <c r="E44" s="46">
         <v>226.63740000000001</v>
       </c>
-      <c r="F44" s="47">
+      <c r="F44" s="46">
         <v>88.545900000000003</v>
       </c>
-      <c r="G44" s="47">
+      <c r="G44" s="46">
         <v>690.1558</v>
       </c>
-      <c r="H44" s="47">
+      <c r="H44" s="46">
         <v>449.1515</v>
       </c>
-      <c r="I44" s="47">
+      <c r="I44" s="46">
         <v>2229.2559000000001</v>
       </c>
-      <c r="J44" s="47">
+      <c r="J44" s="46">
         <v>70.683700000000002</v>
       </c>
-      <c r="K44" s="48">
+      <c r="K44" s="47">
         <f t="shared" si="3"/>
         <v>522.94982886572041</v>
       </c>
@@ -15603,31 +15808,31 @@
       <c r="B45" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="47">
+      <c r="C45" s="46">
         <v>302.92380000000003</v>
       </c>
-      <c r="D45" s="47">
+      <c r="D45" s="46">
         <v>107.7985</v>
       </c>
-      <c r="E45" s="47">
+      <c r="E45" s="46">
         <v>233.28129999999999</v>
       </c>
-      <c r="F45" s="47">
+      <c r="F45" s="46">
         <v>272.55579999999998</v>
       </c>
-      <c r="G45" s="47">
+      <c r="G45" s="46">
         <v>412.64940000000001</v>
       </c>
-      <c r="H45" s="47">
+      <c r="H45" s="46">
         <v>216.39189999999999</v>
       </c>
-      <c r="I45" s="47">
+      <c r="I45" s="46">
         <v>1300.1991</v>
       </c>
-      <c r="J45" s="47">
+      <c r="J45" s="46">
         <v>19.7029</v>
       </c>
-      <c r="K45" s="48">
+      <c r="K45" s="47">
         <f t="shared" si="3"/>
         <v>290.43536469036553</v>
       </c>
@@ -15656,31 +15861,31 @@
       <c r="B46" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="47">
+      <c r="C46" s="46">
         <v>841.48389999999995</v>
       </c>
-      <c r="D46" s="47">
+      <c r="D46" s="46">
         <v>266.28210000000001</v>
       </c>
-      <c r="E46" s="47">
+      <c r="E46" s="46">
         <v>567.08529999999996</v>
       </c>
-      <c r="F46" s="47">
+      <c r="F46" s="46">
         <v>83.794899999999998</v>
       </c>
-      <c r="G46" s="47">
+      <c r="G46" s="46">
         <v>1173.4446</v>
       </c>
-      <c r="H46" s="47">
+      <c r="H46" s="46">
         <v>584.11469999999997</v>
       </c>
-      <c r="I46" s="47">
+      <c r="I46" s="46">
         <v>1689.2844</v>
       </c>
-      <c r="J46" s="47">
+      <c r="J46" s="46">
         <v>69.169899999999998</v>
       </c>
-      <c r="K46" s="48">
+      <c r="K46" s="47">
         <f t="shared" si="3"/>
         <v>671.57220729807807</v>
       </c>
@@ -15709,54 +15914,541 @@
       <c r="B47" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="47">
+      <c r="C47" s="46">
         <v>973.22990000000004</v>
       </c>
-      <c r="D47" s="47">
+      <c r="D47" s="46">
         <v>417.33859999999999</v>
       </c>
-      <c r="E47" s="47">
+      <c r="E47" s="46">
         <v>244.90539999999999</v>
       </c>
-      <c r="F47" s="47">
+      <c r="F47" s="46">
         <v>133.24469999999999</v>
       </c>
-      <c r="G47" s="47">
+      <c r="G47" s="46">
         <v>624.19479999999999</v>
       </c>
-      <c r="H47" s="47">
+      <c r="H47" s="46">
         <v>382.09559999999999</v>
       </c>
-      <c r="I47" s="47">
+      <c r="I47" s="46">
         <v>1069.2180000000001</v>
       </c>
-      <c r="J47" s="47">
+      <c r="J47" s="46">
         <v>64.067099999999996</v>
       </c>
-      <c r="K47" s="48">
+      <c r="K47" s="47">
         <f t="shared" si="3"/>
         <v>523.17066129883187</v>
       </c>
       <c r="M47" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="N47" s="48">
+      <c r="N47" s="47">
         <f>MAX(N35:N46)</f>
         <v>4816.2437586735341</v>
       </c>
-      <c r="O47" s="48">
+      <c r="O47" s="47">
         <f>MAX(O35:O46)</f>
         <v>137.81504300366882</v>
       </c>
     </row>
+    <row r="56" spans="2:12">
+      <c r="B56" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52"/>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="52"/>
+      <c r="J56" s="52"/>
+      <c r="K56" s="52"/>
+      <c r="L56" s="52"/>
+    </row>
+    <row r="57" spans="2:12">
+      <c r="B57" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="E57" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F57" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="G57" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="H57" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="I57" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="J57" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="K57" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="L57" s="42" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12">
+      <c r="B58" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="43">
+        <v>1</v>
+      </c>
+      <c r="D58" s="39">
+        <v>4</v>
+      </c>
+      <c r="E58" s="39">
+        <v>1</v>
+      </c>
+      <c r="F58" s="39">
+        <v>1</v>
+      </c>
+      <c r="G58" s="39">
+        <v>2</v>
+      </c>
+      <c r="H58" s="39">
+        <v>1</v>
+      </c>
+      <c r="I58" s="39">
+        <v>1</v>
+      </c>
+      <c r="J58" s="39">
+        <v>1</v>
+      </c>
+      <c r="K58" s="43">
+        <f t="shared" ref="K58:K69" si="4">SUM(C58:J58)</f>
+        <v>12</v>
+      </c>
+      <c r="L58" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12">
+      <c r="B59" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C59" s="43">
+        <v>4</v>
+      </c>
+      <c r="D59" s="39">
+        <v>3</v>
+      </c>
+      <c r="E59" s="39">
+        <v>2</v>
+      </c>
+      <c r="F59" s="39">
+        <v>2</v>
+      </c>
+      <c r="G59" s="39">
+        <v>3</v>
+      </c>
+      <c r="H59" s="39">
+        <v>2</v>
+      </c>
+      <c r="I59" s="39">
+        <v>2</v>
+      </c>
+      <c r="J59" s="39">
+        <v>2</v>
+      </c>
+      <c r="K59" s="43">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="L59" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12">
+      <c r="B60" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" s="43">
+        <v>7</v>
+      </c>
+      <c r="D60" s="39">
+        <v>1</v>
+      </c>
+      <c r="E60" s="39">
+        <v>4</v>
+      </c>
+      <c r="F60" s="39">
+        <v>6</v>
+      </c>
+      <c r="G60" s="39">
+        <v>1</v>
+      </c>
+      <c r="H60" s="39">
+        <v>4</v>
+      </c>
+      <c r="I60" s="39">
+        <v>3</v>
+      </c>
+      <c r="J60" s="39">
+        <v>3</v>
+      </c>
+      <c r="K60" s="43">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="L60" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12">
+      <c r="B61" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61" s="43">
+        <v>2</v>
+      </c>
+      <c r="D61" s="39">
+        <v>2</v>
+      </c>
+      <c r="E61" s="39">
+        <v>5</v>
+      </c>
+      <c r="F61" s="39">
+        <v>4</v>
+      </c>
+      <c r="G61" s="39">
+        <v>4</v>
+      </c>
+      <c r="H61" s="39">
+        <v>3</v>
+      </c>
+      <c r="I61" s="39">
+        <v>7</v>
+      </c>
+      <c r="J61" s="39">
+        <v>5</v>
+      </c>
+      <c r="K61" s="43">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="L61" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12">
+      <c r="B62" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" s="43">
+        <v>9</v>
+      </c>
+      <c r="D62" s="39">
+        <v>8</v>
+      </c>
+      <c r="E62" s="39">
+        <v>3</v>
+      </c>
+      <c r="F62" s="39">
+        <v>7</v>
+      </c>
+      <c r="G62" s="39">
+        <v>5</v>
+      </c>
+      <c r="H62" s="39">
+        <v>5</v>
+      </c>
+      <c r="I62" s="39">
+        <v>5</v>
+      </c>
+      <c r="J62" s="39">
+        <v>4</v>
+      </c>
+      <c r="K62" s="43">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="L62" s="49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12">
+      <c r="B63" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" s="43">
+        <v>3</v>
+      </c>
+      <c r="D63" s="39">
+        <v>7</v>
+      </c>
+      <c r="E63" s="39">
+        <v>8</v>
+      </c>
+      <c r="F63" s="39">
+        <v>5</v>
+      </c>
+      <c r="G63" s="39">
+        <v>6</v>
+      </c>
+      <c r="H63" s="39">
+        <v>6</v>
+      </c>
+      <c r="I63" s="39">
+        <v>6</v>
+      </c>
+      <c r="J63" s="39">
+        <v>9</v>
+      </c>
+      <c r="K63" s="43">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="L63" s="49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12">
+      <c r="B64" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="43">
+        <v>11</v>
+      </c>
+      <c r="D64" s="39">
+        <v>10</v>
+      </c>
+      <c r="E64" s="39">
+        <v>6</v>
+      </c>
+      <c r="F64" s="39">
+        <v>3</v>
+      </c>
+      <c r="G64" s="39">
+        <v>8</v>
+      </c>
+      <c r="H64" s="39">
+        <v>7</v>
+      </c>
+      <c r="I64" s="39">
+        <v>4</v>
+      </c>
+      <c r="J64" s="39">
+        <v>11</v>
+      </c>
+      <c r="K64" s="43">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="L64" s="49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12">
+      <c r="B65" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C65" s="43">
+        <v>5</v>
+      </c>
+      <c r="D65" s="39">
+        <v>6</v>
+      </c>
+      <c r="E65" s="39">
+        <v>9</v>
+      </c>
+      <c r="F65" s="39">
+        <v>9</v>
+      </c>
+      <c r="G65" s="39">
+        <v>10</v>
+      </c>
+      <c r="H65" s="39">
+        <v>9</v>
+      </c>
+      <c r="I65" s="39">
+        <v>9</v>
+      </c>
+      <c r="J65" s="39">
+        <v>7</v>
+      </c>
+      <c r="K65" s="43">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="L65" s="49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12">
+      <c r="B66" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C66" s="43">
+        <v>8</v>
+      </c>
+      <c r="D66" s="39">
+        <v>9</v>
+      </c>
+      <c r="E66" s="39">
+        <v>7</v>
+      </c>
+      <c r="F66" s="39">
+        <v>10</v>
+      </c>
+      <c r="G66" s="39">
+        <v>7</v>
+      </c>
+      <c r="H66" s="39">
+        <v>8</v>
+      </c>
+      <c r="I66" s="39">
+        <v>8</v>
+      </c>
+      <c r="J66" s="39">
+        <v>8</v>
+      </c>
+      <c r="K66" s="43">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+      <c r="L66" s="49">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12">
+      <c r="B67" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C67" s="43">
+        <v>6</v>
+      </c>
+      <c r="D67" s="39">
+        <v>5</v>
+      </c>
+      <c r="E67" s="39">
+        <v>11</v>
+      </c>
+      <c r="F67" s="39">
+        <v>8</v>
+      </c>
+      <c r="G67" s="39">
+        <v>11</v>
+      </c>
+      <c r="H67" s="39">
+        <v>10</v>
+      </c>
+      <c r="I67" s="39">
+        <v>11</v>
+      </c>
+      <c r="J67" s="39">
+        <v>10</v>
+      </c>
+      <c r="K67" s="43">
+        <f t="shared" si="4"/>
+        <v>72</v>
+      </c>
+      <c r="L67" s="49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12">
+      <c r="B68" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" s="43">
+        <v>12</v>
+      </c>
+      <c r="D68" s="39">
+        <v>11</v>
+      </c>
+      <c r="E68" s="39">
+        <v>10</v>
+      </c>
+      <c r="F68" s="39">
+        <v>11</v>
+      </c>
+      <c r="G68" s="39">
+        <v>9</v>
+      </c>
+      <c r="H68" s="39">
+        <v>11</v>
+      </c>
+      <c r="I68" s="39">
+        <v>10</v>
+      </c>
+      <c r="J68" s="39">
+        <v>6</v>
+      </c>
+      <c r="K68" s="43">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="L68" s="49">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12">
+      <c r="B69" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" s="43">
+        <v>10</v>
+      </c>
+      <c r="D69" s="39">
+        <v>12</v>
+      </c>
+      <c r="E69" s="39">
+        <v>12</v>
+      </c>
+      <c r="F69" s="39">
+        <v>12</v>
+      </c>
+      <c r="G69" s="39">
+        <v>12</v>
+      </c>
+      <c r="H69" s="39">
+        <v>12</v>
+      </c>
+      <c r="I69" s="39">
+        <v>12</v>
+      </c>
+      <c r="J69" s="39">
+        <v>12</v>
+      </c>
+      <c r="K69" s="43">
+        <f t="shared" si="4"/>
+        <v>94</v>
+      </c>
+      <c r="L69" s="49">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12">
+      <c r="K70" s="43"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I15:K26">
-    <sortCondition ref="I14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B58:L69">
+    <sortCondition ref="K57"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A33:J33"/>
+    <mergeCell ref="B56:L56"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
House keeping of 10th July
</commit_message>
<xml_diff>
--- a/data_files/final_dataset_jss/processed_result.xlsx
+++ b/data_files/final_dataset_jss/processed_result.xlsx
@@ -1,27 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdn769\FindCochangeByClone\data_files\final_dataset_jss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3FC79E-784D-4866-BEB9-D203C6EB9CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C339484F-6D53-4947-B748-6E69B944E95A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-4404" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cw_separate_types" sheetId="2" r:id="rId1"/>
     <sheet name="Bar Chart" sheetId="8" r:id="rId2"/>
     <sheet name="Ranking" sheetId="7" r:id="rId3"/>
-    <sheet name="max cochange" sheetId="3" r:id="rId4"/>
-    <sheet name="Data Processed" sheetId="4" r:id="rId5"/>
-    <sheet name="tool configuration" sheetId="5" r:id="rId6"/>
-    <sheet name="Percent Cloned Cochange" sheetId="6" r:id="rId7"/>
-    <sheet name="avg_unique_line_coverage" sheetId="9" r:id="rId8"/>
+    <sheet name="Rank_Wilcoxon" sheetId="10" r:id="rId4"/>
+    <sheet name="max cochange" sheetId="3" r:id="rId5"/>
+    <sheet name="Data Processed" sheetId="4" r:id="rId6"/>
+    <sheet name="tool configuration" sheetId="5" r:id="rId7"/>
+    <sheet name="Percent Cloned Cochange" sheetId="6" r:id="rId8"/>
+    <sheet name="avg_unique_line_coverage" sheetId="9" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Rank_Wilcoxon!$E$17:$E$83</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="174">
   <si>
     <t>ccfinder</t>
   </si>
@@ -554,6 +558,27 @@
   <si>
     <t>Sum of Ranks</t>
   </si>
+  <si>
+    <t>Feature Sets 1</t>
+  </si>
+  <si>
+    <t>Feature Sets 2</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Result (p&lt;0.5)</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
 </sst>
 </file>
 
@@ -704,7 +729,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -838,6 +863,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10947,48 +10984,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41">
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="Q1" s="51" t="s">
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="Q1" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AD1" s="51" t="s">
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="55"/>
+      <c r="AD1" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
+      <c r="AE1" s="55"/>
+      <c r="AF1" s="55"/>
+      <c r="AG1" s="55"/>
+      <c r="AH1" s="55"/>
+      <c r="AI1" s="55"/>
+      <c r="AJ1" s="55"/>
+      <c r="AK1" s="55"/>
+      <c r="AL1" s="55"/>
+      <c r="AM1" s="55"/>
+      <c r="AN1" s="55"/>
+      <c r="AO1" s="55"/>
     </row>
     <row r="2" spans="1:41">
       <c r="A2" s="5" t="s">
@@ -12541,13 +12578,13 @@
       <c r="Y22" s="2"/>
     </row>
     <row r="23" spans="1:25">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
       <c r="R23" s="9" t="s">
         <v>5</v>
       </c>
@@ -12559,13 +12596,13 @@
       <c r="Y23" s="2"/>
     </row>
     <row r="24" spans="1:25">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
       <c r="R24" s="9" t="s">
         <v>7</v>
       </c>
@@ -12577,13 +12614,13 @@
       <c r="Y24" s="2"/>
     </row>
     <row r="25" spans="1:25">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
       <c r="R25" s="9" t="s">
         <v>6</v>
       </c>
@@ -12769,8 +12806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7456461C-E2A3-44D7-A21C-7E2601ED2580}">
   <dimension ref="A1:AN29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="X37" sqref="X37"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T47" sqref="T47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12780,29 +12817,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
       <c r="J1" s="40"/>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="18" t="s">
@@ -13672,8 +13709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB317F8-1811-40BD-9FF4-3B66CC20E864}">
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView topLeftCell="V16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Y43" sqref="Y43"/>
+    <sheetView topLeftCell="A26" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P57" sqref="P57:P69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13688,6 +13725,7 @@
     <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.21875" bestFit="1" customWidth="1"/>
@@ -14243,13 +14281,13 @@
       </c>
     </row>
     <row r="13" spans="1:28">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
     </row>
     <row r="14" spans="1:28">
       <c r="A14" s="16" t="s">
@@ -15221,18 +15259,18 @@
       </c>
     </row>
     <row r="33" spans="1:17">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="B33" s="52"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
     </row>
     <row r="34" spans="1:17">
       <c r="C34" s="18" t="s">
@@ -15954,22 +15992,22 @@
         <v>137.81504300366882</v>
       </c>
     </row>
-    <row r="56" spans="2:12">
-      <c r="B56" s="52" t="s">
+    <row r="56" spans="2:16">
+      <c r="B56" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="C56" s="52"/>
-      <c r="D56" s="52"/>
-      <c r="E56" s="52"/>
-      <c r="F56" s="52"/>
-      <c r="G56" s="52"/>
-      <c r="H56" s="52"/>
-      <c r="I56" s="52"/>
-      <c r="J56" s="52"/>
-      <c r="K56" s="52"/>
-      <c r="L56" s="52"/>
-    </row>
-    <row r="57" spans="2:12">
+      <c r="C56" s="56"/>
+      <c r="D56" s="56"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="56"/>
+      <c r="G56" s="56"/>
+      <c r="H56" s="56"/>
+      <c r="I56" s="56"/>
+      <c r="J56" s="56"/>
+      <c r="K56" s="56"/>
+      <c r="L56" s="56"/>
+    </row>
+    <row r="57" spans="2:16">
       <c r="B57" s="4" t="s">
         <v>109</v>
       </c>
@@ -16003,8 +16041,14 @@
       <c r="L57" s="42" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="58" spans="2:12">
+      <c r="O57" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="P57" s="51" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16">
       <c r="B58" s="4" t="s">
         <v>111</v>
       </c>
@@ -16039,8 +16083,14 @@
       <c r="L58" s="49">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="2:12">
+      <c r="O58" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P58" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16">
       <c r="B59" s="4" t="s">
         <v>112</v>
       </c>
@@ -16075,8 +16125,14 @@
       <c r="L59" s="49">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="2:12">
+      <c r="O59" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="P59" s="49">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16">
       <c r="B60" s="4" t="s">
         <v>48</v>
       </c>
@@ -16111,8 +16167,14 @@
       <c r="L60" s="49">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="2:12">
+      <c r="O60" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="P60" s="49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16">
       <c r="B61" s="4" t="s">
         <v>46</v>
       </c>
@@ -16147,8 +16209,14 @@
       <c r="L61" s="49">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="2:12">
+      <c r="O61" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="P61" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16">
       <c r="B62" s="4" t="s">
         <v>110</v>
       </c>
@@ -16183,8 +16251,14 @@
       <c r="L62" s="49">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="2:12">
+      <c r="O62" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="P62" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16">
       <c r="B63" s="4" t="s">
         <v>47</v>
       </c>
@@ -16219,8 +16293,14 @@
       <c r="L63" s="49">
         <v>6</v>
       </c>
-    </row>
-    <row r="64" spans="2:12">
+      <c r="O63" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="P63" s="49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16">
       <c r="B64" s="4" t="s">
         <v>50</v>
       </c>
@@ -16255,8 +16335,14 @@
       <c r="L64" s="49">
         <v>7</v>
       </c>
-    </row>
-    <row r="65" spans="2:12">
+      <c r="O64" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P64" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="2:16">
       <c r="B65" s="4" t="s">
         <v>53</v>
       </c>
@@ -16291,8 +16377,14 @@
       <c r="L65" s="49">
         <v>8</v>
       </c>
-    </row>
-    <row r="66" spans="2:12">
+      <c r="O65" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="P65" s="49">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="2:16">
       <c r="B66" s="4" t="s">
         <v>51</v>
       </c>
@@ -16327,8 +16419,14 @@
       <c r="L66" s="49">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="2:12">
+      <c r="O66" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P66" s="49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="2:16">
       <c r="B67" s="4" t="s">
         <v>52</v>
       </c>
@@ -16363,8 +16461,14 @@
       <c r="L67" s="49">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="2:12">
+      <c r="O67" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P67" s="49">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="2:16">
       <c r="B68" s="4" t="s">
         <v>113</v>
       </c>
@@ -16399,8 +16503,14 @@
       <c r="L68" s="49">
         <v>11</v>
       </c>
-    </row>
-    <row r="69" spans="2:12">
+      <c r="O68" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="P68" s="49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="2:16">
       <c r="B69" s="4" t="s">
         <v>49</v>
       </c>
@@ -16435,13 +16545,19 @@
       <c r="L69" s="49">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="2:12">
+      <c r="O69" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P69" s="49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="2:16">
       <c r="K70" s="43"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B58:L69">
-    <sortCondition ref="K57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O58:P69">
+    <sortCondition ref="O57"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="A13:E13"/>
@@ -16456,6 +16572,1825 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46015174-E766-4E6A-9E50-9EC594E0B4D4}">
+  <dimension ref="A1:T83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.31619371320508294</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.16207543018844645</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.360817657800581</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.24602546786115667</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.14562871999866411</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.30457568239097665</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.34833551113640071</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.48762200648671372</v>
+      </c>
+      <c r="J3" s="49">
+        <v>1</v>
+      </c>
+      <c r="K3" s="49"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.27181547323372851</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.17861077444078158</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.29065802642113286</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.23699432045688906</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.10887560949091929</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.2013734495507056</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.19940061345749924</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.42220770848218803</v>
+      </c>
+      <c r="J4" s="49">
+        <v>2</v>
+      </c>
+      <c r="K4" s="49"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.18797513965985915</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.57006629342770809</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.20987329560746865</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.1465119856518563</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.29809958472766163</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.1403356572328241</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.18233509152786742</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.40694926295858275</v>
+      </c>
+      <c r="J5" s="49">
+        <v>3</v>
+      </c>
+      <c r="K5" s="49"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.29689219819289236</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.23159638283190104</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.19626765052556303</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.16443768556651236</v>
+      </c>
+      <c r="F6" s="1">
+        <v>8.7077801565042398E-2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.14630424874279643</v>
+      </c>
+      <c r="H6" s="1">
+        <v>7.1766545065928722E-2</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.16445105089370873</v>
+      </c>
+      <c r="J6" s="49">
+        <v>4</v>
+      </c>
+      <c r="K6" s="49"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.13401411223842602</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6.6790752080657587E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.21668514712070192</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.11841284915151483</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8.3757738928440878E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.12704153066461318</v>
+      </c>
+      <c r="H7" s="1">
+        <v>8.1891245921076911E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.1683508020694893</v>
+      </c>
+      <c r="J7" s="49">
+        <v>5</v>
+      </c>
+      <c r="K7" s="49"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.28452072265590272</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.10031116983650794</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.12019674662205297</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.14818895976333404</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7.5293986069825763E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.12153127420312233</v>
+      </c>
+      <c r="H8" s="1">
+        <v>8.3527580112865291E-2</v>
+      </c>
+      <c r="I8" s="1">
+        <v>7.6748667238038124E-2</v>
+      </c>
+      <c r="J8" s="49">
+        <v>6</v>
+      </c>
+      <c r="K8" s="49"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.2601238370710906</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.1463441385744782</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8.1060017209975452E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8.1238618461740797E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3.0822297402631649E-2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>8.7290938644931079E-2</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4.9527655219623268E-2</v>
+      </c>
+      <c r="I9" s="1">
+        <v>9.676763458695227E-2</v>
+      </c>
+      <c r="J9" s="49">
+        <v>7</v>
+      </c>
+      <c r="K9" s="49"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.2474800252749117</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.15560731711942238</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6.4937795734906031E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.10796217631724295</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.8889941659942939E-2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>6.8331761752691206E-2</v>
+      </c>
+      <c r="H10" s="1">
+        <v>3.2749663794473464E-2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>5.6638671002405841E-2</v>
+      </c>
+      <c r="J10" s="49">
+        <v>8</v>
+      </c>
+      <c r="K10" s="49"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.12333801778239918</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6.1618928714424016E-2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.15810764408345859</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.2070328019427411</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3.5612743058776548E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.10400836731617218</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.12308705162242017</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3.0178201729187566E-2</v>
+      </c>
+      <c r="J11" s="49">
+        <v>9</v>
+      </c>
+      <c r="K11" s="49"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.16516261855866468</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6.5278366659934667E-2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.15025783750484722</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4.4244091320165067E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4.6520155384710847E-2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.10017098457498899</v>
+      </c>
+      <c r="H12" s="1">
+        <v>6.4074139851070161E-2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>9.7487222735909748E-2</v>
+      </c>
+      <c r="J12" s="49">
+        <v>10</v>
+      </c>
+      <c r="K12" s="49"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="1">
+        <v>9.3598732380710842E-2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.5430717389884875E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5.8442489421290759E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3.0245059081465474E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3.0165628809702718E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>4.7011643764859522E-2</v>
+      </c>
+      <c r="H13" s="1">
+        <v>3.5661492889273186E-2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.1115247322914209</v>
+      </c>
+      <c r="J13" s="49">
+        <v>11</v>
+      </c>
+      <c r="K13" s="49"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.11813878657280781</v>
+      </c>
+      <c r="C14" s="1">
+        <v>8.96091620790441E-3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3.1027797949163761E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3.2909728197061942E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.0931634311275707E-2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2.2808896210375261E-2</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>4.7581278634266687E-3</v>
+      </c>
+      <c r="J14" s="49">
+        <v>12</v>
+      </c>
+      <c r="K14" s="49"/>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="D17" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="I17" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="J17" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="56"/>
+      <c r="T17" s="52" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="53">
+        <v>2</v>
+      </c>
+      <c r="D18" s="53">
+        <v>2.4883994999999999E-2</v>
+      </c>
+      <c r="E18" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="I18" t="s">
+        <v>111</v>
+      </c>
+      <c r="J18" t="s">
+        <v>112</v>
+      </c>
+      <c r="K18" t="s">
+        <v>46</v>
+      </c>
+      <c r="L18" t="s">
+        <v>110</v>
+      </c>
+      <c r="M18" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18" t="s">
+        <v>50</v>
+      </c>
+      <c r="O18" t="s">
+        <v>53</v>
+      </c>
+      <c r="P18" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>52</v>
+      </c>
+      <c r="R18" t="s">
+        <v>113</v>
+      </c>
+      <c r="S18" t="s">
+        <v>49</v>
+      </c>
+      <c r="T18" s="53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="53">
+        <v>12.5</v>
+      </c>
+      <c r="D19" s="53">
+        <v>0.44064789700000001</v>
+      </c>
+      <c r="E19" s="53">
+        <v>-1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>112</v>
+      </c>
+      <c r="J19" t="s">
+        <v>110</v>
+      </c>
+      <c r="K19" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19" t="s">
+        <v>53</v>
+      </c>
+      <c r="N19" t="s">
+        <v>51</v>
+      </c>
+      <c r="O19" t="s">
+        <v>52</v>
+      </c>
+      <c r="P19" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>49</v>
+      </c>
+      <c r="T19" s="53">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="53">
+        <v>3</v>
+      </c>
+      <c r="D20" s="53">
+        <v>3.5691899999999999E-2</v>
+      </c>
+      <c r="E20" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="I20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" t="s">
+        <v>110</v>
+      </c>
+      <c r="K20" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" t="s">
+        <v>53</v>
+      </c>
+      <c r="M20" t="s">
+        <v>51</v>
+      </c>
+      <c r="N20" t="s">
+        <v>52</v>
+      </c>
+      <c r="O20" t="s">
+        <v>113</v>
+      </c>
+      <c r="P20" t="s">
+        <v>49</v>
+      </c>
+      <c r="T20" s="53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="53">
+        <v>0</v>
+      </c>
+      <c r="D21" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="I21" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" t="s">
+        <v>47</v>
+      </c>
+      <c r="K21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" t="s">
+        <v>53</v>
+      </c>
+      <c r="M21" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" t="s">
+        <v>113</v>
+      </c>
+      <c r="O21" t="s">
+        <v>49</v>
+      </c>
+      <c r="T21" s="53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="53">
+        <v>0</v>
+      </c>
+      <c r="D22" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="I22" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22" t="s">
+        <v>113</v>
+      </c>
+      <c r="K22" t="s">
+        <v>49</v>
+      </c>
+      <c r="T22" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="53">
+        <v>0</v>
+      </c>
+      <c r="D23" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="I23" t="s">
+        <v>47</v>
+      </c>
+      <c r="J23" t="s">
+        <v>113</v>
+      </c>
+      <c r="K23" t="s">
+        <v>49</v>
+      </c>
+      <c r="T23" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="53">
+        <v>0</v>
+      </c>
+      <c r="D24" s="53">
+        <v>1.7960477999999998E-2</v>
+      </c>
+      <c r="E24" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="I24" t="s">
+        <v>50</v>
+      </c>
+      <c r="J24" t="s">
+        <v>113</v>
+      </c>
+      <c r="K24" t="s">
+        <v>49</v>
+      </c>
+      <c r="T24" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="53">
+        <v>0</v>
+      </c>
+      <c r="D25" s="53">
+        <v>1.1616045E-2</v>
+      </c>
+      <c r="E25" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="I25" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" t="s">
+        <v>49</v>
+      </c>
+      <c r="T25" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="53">
+        <v>0</v>
+      </c>
+      <c r="D26" s="53">
+        <v>1.1616045E-2</v>
+      </c>
+      <c r="E26" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="I26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" t="s">
+        <v>49</v>
+      </c>
+      <c r="T26" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="53">
+        <v>0</v>
+      </c>
+      <c r="D27" s="53">
+        <v>1.1616045E-2</v>
+      </c>
+      <c r="E27" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="I27" t="s">
+        <v>52</v>
+      </c>
+      <c r="J27" t="s">
+        <v>113</v>
+      </c>
+      <c r="K27" t="s">
+        <v>49</v>
+      </c>
+      <c r="T27" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="53">
+        <v>0</v>
+      </c>
+      <c r="D28" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E28" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="53">
+        <v>15</v>
+      </c>
+      <c r="D29" s="53">
+        <v>0.67442407199999999</v>
+      </c>
+      <c r="E29" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="53">
+        <v>5.5</v>
+      </c>
+      <c r="D30" s="53">
+        <v>7.9688025999999995E-2</v>
+      </c>
+      <c r="E30" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="53">
+        <v>0</v>
+      </c>
+      <c r="D31" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E31" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="53">
+        <v>1</v>
+      </c>
+      <c r="D32" s="53">
+        <v>1.7290281000000001E-2</v>
+      </c>
+      <c r="E32" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="53">
+        <v>0</v>
+      </c>
+      <c r="D33" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E33" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="53">
+        <v>0</v>
+      </c>
+      <c r="D34" s="53">
+        <v>1.1616045E-2</v>
+      </c>
+      <c r="E34" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="53">
+        <v>0</v>
+      </c>
+      <c r="D35" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E35" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="53">
+        <v>0</v>
+      </c>
+      <c r="D36" s="53">
+        <v>1.1616045E-2</v>
+      </c>
+      <c r="E36" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="53">
+        <v>0</v>
+      </c>
+      <c r="D37" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E37" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="53">
+        <v>0</v>
+      </c>
+      <c r="D38" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E38" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="53">
+        <v>9</v>
+      </c>
+      <c r="D39" s="53">
+        <v>0.206462587</v>
+      </c>
+      <c r="E39" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="53">
+        <v>1.5</v>
+      </c>
+      <c r="D40" s="53">
+        <v>2.0706216E-2</v>
+      </c>
+      <c r="E40" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="53">
+        <v>3</v>
+      </c>
+      <c r="D41" s="53">
+        <v>6.2979050999999994E-2</v>
+      </c>
+      <c r="E41" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="53">
+        <v>3</v>
+      </c>
+      <c r="D42" s="53">
+        <v>3.5465864999999999E-2</v>
+      </c>
+      <c r="E42" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="53">
+        <v>2</v>
+      </c>
+      <c r="D43" s="53">
+        <v>2.4883994999999999E-2</v>
+      </c>
+      <c r="E43" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="53">
+        <v>3.5</v>
+      </c>
+      <c r="D44" s="53">
+        <v>4.2062732999999998E-2</v>
+      </c>
+      <c r="E44" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="53">
+        <v>0</v>
+      </c>
+      <c r="D45" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E45" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="53">
+        <v>0</v>
+      </c>
+      <c r="D46" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E46" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="53">
+        <v>0</v>
+      </c>
+      <c r="D47" s="53">
+        <v>1.1616045E-2</v>
+      </c>
+      <c r="E47" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>110</v>
+      </c>
+      <c r="C48" s="53">
+        <v>9</v>
+      </c>
+      <c r="D48" s="53">
+        <v>0.206462587</v>
+      </c>
+      <c r="E48" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="53">
+        <v>1.5</v>
+      </c>
+      <c r="D49" s="53">
+        <v>2.0706216E-2</v>
+      </c>
+      <c r="E49" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="53">
+        <v>0</v>
+      </c>
+      <c r="D50" s="53">
+        <v>1.1310671E-2</v>
+      </c>
+      <c r="E50" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="53">
+        <v>0</v>
+      </c>
+      <c r="D51" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E51" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="53">
+        <v>6</v>
+      </c>
+      <c r="D52" s="53">
+        <v>9.128957E-2</v>
+      </c>
+      <c r="E52" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="53">
+        <v>0</v>
+      </c>
+      <c r="D53" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E53" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" s="53">
+        <v>0</v>
+      </c>
+      <c r="D54" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E54" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" t="s">
+        <v>49</v>
+      </c>
+      <c r="C55" s="53">
+        <v>0</v>
+      </c>
+      <c r="D55" s="53">
+        <v>1.1616045E-2</v>
+      </c>
+      <c r="E55" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="53">
+        <v>10</v>
+      </c>
+      <c r="D56" s="53">
+        <v>0.916282441</v>
+      </c>
+      <c r="E56" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" s="53">
+        <v>13</v>
+      </c>
+      <c r="D57" s="53">
+        <v>0.48383985099999999</v>
+      </c>
+      <c r="E57" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" s="53">
+        <v>12</v>
+      </c>
+      <c r="D58" s="53">
+        <v>0.40023614400000002</v>
+      </c>
+      <c r="E58" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" s="53">
+        <v>11</v>
+      </c>
+      <c r="D59" s="53">
+        <v>0.326395777</v>
+      </c>
+      <c r="E59" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" s="53">
+        <v>4</v>
+      </c>
+      <c r="D60" s="53">
+        <v>8.9814344000000004E-2</v>
+      </c>
+      <c r="E60" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" t="s">
+        <v>113</v>
+      </c>
+      <c r="C61" s="53">
+        <v>0</v>
+      </c>
+      <c r="D61" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E61" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" t="s">
+        <v>49</v>
+      </c>
+      <c r="C62" s="53">
+        <v>0</v>
+      </c>
+      <c r="D62" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E62" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" s="53">
+        <v>7</v>
+      </c>
+      <c r="D63" s="53">
+        <v>0.123025194</v>
+      </c>
+      <c r="E63" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" t="s">
+        <v>53</v>
+      </c>
+      <c r="C64" s="53">
+        <v>7.5</v>
+      </c>
+      <c r="D64" s="53">
+        <v>0.14050554100000001</v>
+      </c>
+      <c r="E64" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B65" t="s">
+        <v>51</v>
+      </c>
+      <c r="C65" s="53">
+        <v>13.5</v>
+      </c>
+      <c r="D65" s="53">
+        <v>0.52810612499999998</v>
+      </c>
+      <c r="E65" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66" t="s">
+        <v>52</v>
+      </c>
+      <c r="C66" s="53">
+        <v>7.5</v>
+      </c>
+      <c r="D66" s="53">
+        <v>0.139036939</v>
+      </c>
+      <c r="E66" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>47</v>
+      </c>
+      <c r="B67" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" s="53">
+        <v>1</v>
+      </c>
+      <c r="D67" s="53">
+        <v>1.7290281000000001E-2</v>
+      </c>
+      <c r="E67" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>47</v>
+      </c>
+      <c r="B68" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" s="53">
+        <v>0</v>
+      </c>
+      <c r="D68" s="53">
+        <v>1.1616045E-2</v>
+      </c>
+      <c r="E68" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>50</v>
+      </c>
+      <c r="B69" t="s">
+        <v>53</v>
+      </c>
+      <c r="C69" s="53">
+        <v>7.5</v>
+      </c>
+      <c r="D69" s="53">
+        <v>0.27018109600000001</v>
+      </c>
+      <c r="E69" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>50</v>
+      </c>
+      <c r="B70" t="s">
+        <v>51</v>
+      </c>
+      <c r="C70" s="53">
+        <v>18</v>
+      </c>
+      <c r="D70" s="53">
+        <v>1</v>
+      </c>
+      <c r="E70" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>50</v>
+      </c>
+      <c r="B71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C71" s="53">
+        <v>11</v>
+      </c>
+      <c r="D71" s="53">
+        <v>0.61208987999999998</v>
+      </c>
+      <c r="E71" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B72" t="s">
+        <v>113</v>
+      </c>
+      <c r="C72" s="53">
+        <v>1</v>
+      </c>
+      <c r="D72" s="53">
+        <v>2.7991815E-2</v>
+      </c>
+      <c r="E72" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" t="s">
+        <v>49</v>
+      </c>
+      <c r="C73" s="53">
+        <v>0</v>
+      </c>
+      <c r="D73" s="53">
+        <v>1.1310671E-2</v>
+      </c>
+      <c r="E73" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>53</v>
+      </c>
+      <c r="B74" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74" s="53">
+        <v>17</v>
+      </c>
+      <c r="D74" s="53">
+        <v>0.88836569899999995</v>
+      </c>
+      <c r="E74" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>53</v>
+      </c>
+      <c r="B75" t="s">
+        <v>52</v>
+      </c>
+      <c r="C75" s="53">
+        <v>17.5</v>
+      </c>
+      <c r="D75" s="53">
+        <v>0.94404542599999997</v>
+      </c>
+      <c r="E75" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76" t="s">
+        <v>113</v>
+      </c>
+      <c r="C76" s="53">
+        <v>4</v>
+      </c>
+      <c r="D76" s="53">
+        <v>0.17295491800000001</v>
+      </c>
+      <c r="E76" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>53</v>
+      </c>
+      <c r="B77" t="s">
+        <v>49</v>
+      </c>
+      <c r="C77" s="53">
+        <v>0</v>
+      </c>
+      <c r="D77" s="53">
+        <v>1.1616045E-2</v>
+      </c>
+      <c r="E77" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>51</v>
+      </c>
+      <c r="B78" t="s">
+        <v>52</v>
+      </c>
+      <c r="C78" s="53">
+        <v>13.5</v>
+      </c>
+      <c r="D78" s="53">
+        <v>0.93252632999999996</v>
+      </c>
+      <c r="E78" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>51</v>
+      </c>
+      <c r="B79" t="s">
+        <v>113</v>
+      </c>
+      <c r="C79" s="53">
+        <v>6</v>
+      </c>
+      <c r="D79" s="53">
+        <v>9.2891941000000006E-2</v>
+      </c>
+      <c r="E79" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>51</v>
+      </c>
+      <c r="B80" t="s">
+        <v>49</v>
+      </c>
+      <c r="C80" s="53">
+        <v>0</v>
+      </c>
+      <c r="D80" s="53">
+        <v>1.7755923E-2</v>
+      </c>
+      <c r="E80" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>52</v>
+      </c>
+      <c r="B81" t="s">
+        <v>113</v>
+      </c>
+      <c r="C81" s="53">
+        <v>1</v>
+      </c>
+      <c r="D81" s="53">
+        <v>1.7290281000000001E-2</v>
+      </c>
+      <c r="E81" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>52</v>
+      </c>
+      <c r="B82" t="s">
+        <v>49</v>
+      </c>
+      <c r="C82" s="53">
+        <v>0</v>
+      </c>
+      <c r="D82" s="53">
+        <v>1.1718686000000001E-2</v>
+      </c>
+      <c r="E82" s="53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>113</v>
+      </c>
+      <c r="B83" t="s">
+        <v>49</v>
+      </c>
+      <c r="C83" s="53">
+        <v>3</v>
+      </c>
+      <c r="D83" s="53">
+        <v>6.1100929999999998E-2</v>
+      </c>
+      <c r="E83" s="53">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="E17:E83" xr:uid="{BEA61A31-5D14-414B-87C5-0D47B1111BA9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J14">
+    <sortCondition ref="J2"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J17:S17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755CB0E3-6498-47B1-B478-E9DCBB7D7A8F}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -16476,7 +18411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1163D3CD-3CD4-434D-AB76-3C63CE8DC544}">
   <dimension ref="A1:M12"/>
   <sheetViews>
@@ -16638,7 +18573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F355F6E9-2619-4B6B-81D2-B0650142961E}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -16804,7 +18739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306950A7-0280-48DD-A788-AA88FF1C9BAB}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -17022,7 +18957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED2D4F5-7A16-487A-AF43-6CC11CF437FA}">
   <dimension ref="A1:P97"/>
   <sheetViews>

</xml_diff>

<commit_message>
Filtered the source meter study in the thesis and also updated the journal paper by adding wilcoxon rank test description
</commit_message>
<xml_diff>
--- a/data_files/final_dataset_jss/processed_result.xlsx
+++ b/data_files/final_dataset_jss/processed_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdn769\FindCochangeByClone\data_files\final_dataset_jss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C339484F-6D53-4947-B748-6E69B944E95A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FCF20D-8144-42FF-870D-F42B81FBD264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="177">
   <si>
     <t>ccfinder</t>
   </si>
@@ -578,6 +578,15 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>Significance Test Result (Wilcoxon Signed Rank Test at p&lt;0.05)</t>
+  </si>
+  <si>
+    <t>Tool in Investigation</t>
+  </si>
+  <si>
+    <t>Significantly Better than the Tools</t>
   </si>
 </sst>
 </file>
@@ -16573,10 +16582,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46015174-E766-4E6A-9E50-9EC594E0B4D4}">
-  <dimension ref="A1:T83"/>
+  <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16591,10 +16600,19 @@
     <col min="8" max="8" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:23">
       <c r="B1" s="56" t="s">
         <v>108</v>
       </c>
@@ -16605,8 +16623,22 @@
       <c r="G1" s="56"/>
       <c r="H1" s="56"/>
       <c r="I1" s="56"/>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="55" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -16638,8 +16670,26 @@
         <v>157</v>
       </c>
       <c r="K2" s="51"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="52" t="s">
+        <v>175</v>
+      </c>
+      <c r="M2" s="55" t="s">
+        <v>176</v>
+      </c>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="52" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -16671,8 +16721,44 @@
         <v>1</v>
       </c>
       <c r="K3" s="49"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M3" t="s">
+        <v>112</v>
+      </c>
+      <c r="N3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" t="s">
+        <v>110</v>
+      </c>
+      <c r="P3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" t="s">
+        <v>53</v>
+      </c>
+      <c r="S3" t="s">
+        <v>51</v>
+      </c>
+      <c r="T3" t="s">
+        <v>52</v>
+      </c>
+      <c r="U3" t="s">
+        <v>113</v>
+      </c>
+      <c r="V3" t="s">
+        <v>49</v>
+      </c>
+      <c r="W3" s="53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -16704,8 +16790,38 @@
         <v>2</v>
       </c>
       <c r="K4" s="49"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4" t="s">
+        <v>112</v>
+      </c>
+      <c r="M4" t="s">
+        <v>110</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" t="s">
+        <v>52</v>
+      </c>
+      <c r="S4" t="s">
+        <v>113</v>
+      </c>
+      <c r="T4" t="s">
+        <v>49</v>
+      </c>
+      <c r="W4" s="53">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -16737,8 +16853,35 @@
         <v>3</v>
       </c>
       <c r="K5" s="49"/>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" t="s">
+        <v>110</v>
+      </c>
+      <c r="N5" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R5" t="s">
+        <v>113</v>
+      </c>
+      <c r="S5" t="s">
+        <v>49</v>
+      </c>
+      <c r="W5" s="53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -16770,8 +16913,32 @@
         <v>4</v>
       </c>
       <c r="K6" s="49"/>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>113</v>
+      </c>
+      <c r="R6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W6" s="53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>110</v>
       </c>
@@ -16803,8 +16970,20 @@
         <v>5</v>
       </c>
       <c r="K7" s="49"/>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" t="s">
+        <v>110</v>
+      </c>
+      <c r="M7" t="s">
+        <v>113</v>
+      </c>
+      <c r="N7" t="s">
+        <v>49</v>
+      </c>
+      <c r="W7" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -16836,8 +17015,20 @@
         <v>6</v>
       </c>
       <c r="K8" s="49"/>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N8" t="s">
+        <v>49</v>
+      </c>
+      <c r="W8" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -16869,8 +17060,20 @@
         <v>7</v>
       </c>
       <c r="K9" s="49"/>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" t="s">
+        <v>113</v>
+      </c>
+      <c r="N9" t="s">
+        <v>49</v>
+      </c>
+      <c r="W9" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -16902,8 +17105,17 @@
         <v>8</v>
       </c>
       <c r="K10" s="49"/>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" t="s">
+        <v>49</v>
+      </c>
+      <c r="W10" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -16935,8 +17147,17 @@
         <v>9</v>
       </c>
       <c r="K11" s="49"/>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" t="s">
+        <v>49</v>
+      </c>
+      <c r="W11" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -16968,8 +17189,20 @@
         <v>10</v>
       </c>
       <c r="K12" s="49"/>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" t="s">
+        <v>113</v>
+      </c>
+      <c r="N12" t="s">
+        <v>49</v>
+      </c>
+      <c r="W12" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
         <v>113</v>
       </c>
@@ -17002,7 +17235,7 @@
       </c>
       <c r="K13" s="49"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -17035,7 +17268,7 @@
       </c>
       <c r="K14" s="49"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:6">
       <c r="A17" s="52" t="s">
         <v>167</v>
       </c>
@@ -17052,26 +17285,8 @@
         <v>171</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="I17" s="52" t="s">
-        <v>167</v>
-      </c>
-      <c r="J17" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="56"/>
-      <c r="P17" s="56"/>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="56"/>
-      <c r="S17" s="56"/>
-      <c r="T17" s="52" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -17087,44 +17302,8 @@
       <c r="E18" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="I18" t="s">
-        <v>111</v>
-      </c>
-      <c r="J18" t="s">
-        <v>112</v>
-      </c>
-      <c r="K18" t="s">
-        <v>46</v>
-      </c>
-      <c r="L18" t="s">
-        <v>110</v>
-      </c>
-      <c r="M18" t="s">
-        <v>47</v>
-      </c>
-      <c r="N18" t="s">
-        <v>50</v>
-      </c>
-      <c r="O18" t="s">
-        <v>53</v>
-      </c>
-      <c r="P18" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>52</v>
-      </c>
-      <c r="R18" t="s">
-        <v>113</v>
-      </c>
-      <c r="S18" t="s">
-        <v>49</v>
-      </c>
-      <c r="T18" s="53">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>111</v>
       </c>
@@ -17140,38 +17319,8 @@
       <c r="E19" s="53">
         <v>-1</v>
       </c>
-      <c r="I19" t="s">
-        <v>112</v>
-      </c>
-      <c r="J19" t="s">
-        <v>110</v>
-      </c>
-      <c r="K19" t="s">
-        <v>47</v>
-      </c>
-      <c r="L19" t="s">
-        <v>50</v>
-      </c>
-      <c r="M19" t="s">
-        <v>53</v>
-      </c>
-      <c r="N19" t="s">
-        <v>51</v>
-      </c>
-      <c r="O19" t="s">
-        <v>52</v>
-      </c>
-      <c r="P19" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>49</v>
-      </c>
-      <c r="T19" s="53">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>111</v>
       </c>
@@ -17187,35 +17336,8 @@
       <c r="E20" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="I20" t="s">
-        <v>48</v>
-      </c>
-      <c r="J20" t="s">
-        <v>110</v>
-      </c>
-      <c r="K20" t="s">
-        <v>50</v>
-      </c>
-      <c r="L20" t="s">
-        <v>53</v>
-      </c>
-      <c r="M20" t="s">
-        <v>51</v>
-      </c>
-      <c r="N20" t="s">
-        <v>52</v>
-      </c>
-      <c r="O20" t="s">
-        <v>113</v>
-      </c>
-      <c r="P20" t="s">
-        <v>49</v>
-      </c>
-      <c r="T20" s="53">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>111</v>
       </c>
@@ -17231,32 +17353,8 @@
       <c r="E21" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="I21" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" t="s">
-        <v>47</v>
-      </c>
-      <c r="K21" t="s">
-        <v>50</v>
-      </c>
-      <c r="L21" t="s">
-        <v>53</v>
-      </c>
-      <c r="M21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N21" t="s">
-        <v>113</v>
-      </c>
-      <c r="O21" t="s">
-        <v>49</v>
-      </c>
-      <c r="T21" s="53">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -17272,20 +17370,8 @@
       <c r="E22" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="I22" t="s">
-        <v>110</v>
-      </c>
-      <c r="J22" t="s">
-        <v>113</v>
-      </c>
-      <c r="K22" t="s">
-        <v>49</v>
-      </c>
-      <c r="T22" s="53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>111</v>
       </c>
@@ -17301,20 +17387,8 @@
       <c r="E23" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="I23" t="s">
-        <v>47</v>
-      </c>
-      <c r="J23" t="s">
-        <v>113</v>
-      </c>
-      <c r="K23" t="s">
-        <v>49</v>
-      </c>
-      <c r="T23" s="53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -17330,20 +17404,8 @@
       <c r="E24" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="I24" t="s">
-        <v>50</v>
-      </c>
-      <c r="J24" t="s">
-        <v>113</v>
-      </c>
-      <c r="K24" t="s">
-        <v>49</v>
-      </c>
-      <c r="T24" s="53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -17359,17 +17421,8 @@
       <c r="E25" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="I25" t="s">
-        <v>53</v>
-      </c>
-      <c r="J25" t="s">
-        <v>49</v>
-      </c>
-      <c r="T25" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20">
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -17385,17 +17438,8 @@
       <c r="E26" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="I26" t="s">
-        <v>51</v>
-      </c>
-      <c r="J26" t="s">
-        <v>49</v>
-      </c>
-      <c r="T26" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20">
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>111</v>
       </c>
@@ -17411,20 +17455,8 @@
       <c r="E27" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="I27" t="s">
-        <v>52</v>
-      </c>
-      <c r="J27" t="s">
-        <v>113</v>
-      </c>
-      <c r="K27" t="s">
-        <v>49</v>
-      </c>
-      <c r="T27" s="53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20">
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -17441,7 +17473,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -17458,7 +17490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -17475,7 +17507,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>112</v>
       </c>
@@ -17492,7 +17524,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -18381,9 +18413,10 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J14">
     <sortCondition ref="J2"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J17:S17"/>
+    <mergeCell ref="M2:V2"/>
+    <mergeCell ref="L1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Build the JSS submitting version online
</commit_message>
<xml_diff>
--- a/data_files/final_dataset_jss/processed_result.xlsx
+++ b/data_files/final_dataset_jss/processed_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdn769\FindCochangeByClone\data_files\final_dataset_jss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FCF20D-8144-42FF-870D-F42B81FBD264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C4040F-7263-4850-BEF9-7685EE441BED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-4404" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cw_separate_types" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="185">
   <si>
     <t>ccfinder</t>
   </si>
@@ -523,9 +523,6 @@
     <t>% of Clone Fragments</t>
   </si>
   <si>
-    <t xml:space="preserve"> % of Line Coverage by Clone Fragments</t>
-  </si>
-  <si>
     <t>Ranking based on sum of ranks in individual systems</t>
   </si>
   <si>
@@ -588,11 +585,41 @@
   <si>
     <t>Significantly Better than the Tools</t>
   </si>
+  <si>
+    <t>Differences</t>
+  </si>
+  <si>
+    <t>Tool-1</t>
+  </si>
+  <si>
+    <t>Tool-2</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rank </t>
+  </si>
+  <si>
+    <t>CLW(T2B)</t>
+  </si>
+  <si>
+    <t>CLW(T3P)</t>
+  </si>
+  <si>
+    <t>CLW(T3T)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> % of Line Coverage by the Clone Fragments</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="15">
     <font>
       <sz val="11"/>
@@ -738,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -885,6 +912,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1045,13 +1084,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -1176,13 +1215,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -1307,13 +1346,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -1438,13 +1477,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -1569,13 +1608,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -1700,13 +1739,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -1836,13 +1875,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -1961,13 +2000,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -2379,13 +2418,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -2510,13 +2549,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -2641,13 +2680,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -2772,13 +2811,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -2903,13 +2942,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -3034,13 +3073,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -3170,13 +3209,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -3306,13 +3345,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -3716,13 +3755,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -3842,13 +3881,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -3968,13 +4007,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -4094,13 +4133,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -4220,13 +4259,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -4346,13 +4385,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -4472,13 +4511,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -4598,13 +4637,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -4682,6 +4721,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4912,7 +4952,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4944,7 +4984,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5010,13 +5050,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -5136,13 +5176,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -5262,13 +5302,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -5388,13 +5428,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -5514,13 +5554,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -5640,13 +5680,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -5766,13 +5806,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -5892,13 +5932,13 @@
                   <c:v>CLW(T1)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CLW(T2Blind)</c:v>
+                  <c:v>CLW(T2B)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CLW(T3Pattern)</c:v>
+                  <c:v>CLW(T3P)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CLW(T3Token)</c:v>
+                  <c:v>CLW(T3T)</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>ConQAT</c:v>
@@ -5976,6 +6016,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -6031,7 +6072,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6090,7 +6131,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6132,7 +6173,1012 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr rot="0" vert="horz"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="2000"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2880" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Ranking!$P$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% of Clone Fragments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Ranking!$M$35:$M$46</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>CCFinder</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CLW(T1)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CLW(T2B)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CLW(T3P)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CLW(T3T)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ConQAT</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Deckard</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Duplo</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>iClones</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nicad</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SimCAD</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Simian</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Ranking!$P$35:$P$46</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.71123523002346156</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26717578396614561</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51187814913004048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90877226297031088</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46409952247480563</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2812934961487919</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0000506143425112</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.216184303379307E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.10858592792062301</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.0306346488863273E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.13944605633265741</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1086317818311528</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-610F-4F17-90DC-CBDDCDDAB084}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Ranking!$Q$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> % of Line Coverage by the Clone Fragments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Ranking!$M$35:$M$46</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>CCFinder</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CLW(T1)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CLW(T2B)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CLW(T3P)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CLW(T3T)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ConQAT</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Deckard</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Duplo</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>iClones</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nicad</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SimCAD</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Simian</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Ranking!$Q$35:$Q$46</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.58443163368435114</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.42220653783694323</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56073978047964834</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81173901081784716</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72651488926163699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.70865390461025268</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99865973191064361</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.49232593448402112</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6899268468769435</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.73566888907853401</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.64604618069921604</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.51192708233551243</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-610F-4F17-90DC-CBDDCDDAB084}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1205791232"/>
+        <c:axId val="865018976"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Ranking!$N$34</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>WA</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Ranking!$M$35:$M$46</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>CCFinder</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>CLW(T1)</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>CLW(T2B)</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>CLW(T3P)</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>CLW(T3T)</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>ConQAT</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Deckard</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Duplo</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>iClones</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Nicad</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>SimCAD</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>Simian</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Ranking!$N$35:$N$46</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>3425.3088677929909</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1286.7185755809573</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2465.2051662102749</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4376.6472184650174</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2235.1033002386639</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1354.7094774525817</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>4816.2437586735341</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>203.05143605074741</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>522.94982886572041</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>290.43536469036553</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>671.57220729807807</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>523.17066129883187</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-610F-4F17-90DC-CBDDCDDAB084}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Ranking!$O$34</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>LineCoveragee</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Ranking!$M$35:$M$46</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>CCFinder</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>CLW(T1)</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>CLW(T2B)</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>CLW(T3P)</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>CLW(T3T)</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>ConQAT</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Deckard</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Duplo</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>iClones</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Nicad</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>SimCAD</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>Simian</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Ranking!$O$35:$O$46</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>80.651565448440451</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>58.264502221498162</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>77.382089706191465</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>112.01998349286291</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>100.2590547181059</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>97.794238836214873</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>137.81504300366882</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>67.940978958794915</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>95.209904869018203</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>101.52230669283769</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>89.154372936491811</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>70.645937362300714</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-610F-4F17-90DC-CBDDCDDAB084}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1205791232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="865018976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="865018976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1205791232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -6172,572 +7218,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1800"/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ranking!$P$34</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>% of Clone Fragments</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:alpha val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Ranking!$M$35:$M$46</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>CCFinder</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>CLW(Type1)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>CLW(2Blind)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>CLW(3Pattern)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>CLW(3Token)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>ConQAT</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Deckard</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Duplo</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>iClones</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Nicad</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>SimCAD</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Simian</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Ranking!$P$35:$P$46</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.71123523002346156</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.26717578396614561</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.51187814913004048</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.90877226297031088</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.46409952247480563</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.2812934961487919</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0000506143425112</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.216184303379307E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.10858592792062301</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.0306346488863273E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.13944605633265741</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.1086317818311528</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-810F-4E56-A6FD-9F65D8387750}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ranking!$Q$34</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v> % of Line Coverage by Clone Fragments</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:alpha val="20000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Ranking!$M$35:$M$46</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>CCFinder</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>CLW(Type1)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>CLW(2Blind)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>CLW(3Pattern)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>CLW(3Token)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>ConQAT</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Deckard</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Duplo</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>iClones</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Nicad</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>SimCAD</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Simian</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Ranking!$Q$35:$Q$46</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.58443163368435114</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.42220653783694323</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.56073978047964834</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.81173901081784716</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.72651488926163699</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.70865390461025268</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.99865973191064361</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.49232593448402112</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.6899268468769435</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.73566888907853401</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.64604618069921604</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.51192708233551243</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-810F-4E56-A6FD-9F65D8387750}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="outEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="444"/>
-        <c:overlap val="-90"/>
-        <c:axId val="810282464"/>
-        <c:axId val="488071808"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="810282464"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="488071808"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="488071808"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="810282464"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="lt1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="3200"/>
+        <a:defRPr sz="2400"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -9401,7 +9882,7 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -9412,7 +9893,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -9435,18 +9916,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="bg1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -9458,7 +9939,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -9466,14 +9947,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
-    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -9505,45 +9983,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -9555,34 +10023,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -9604,13 +10068,15 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -9625,15 +10091,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -9644,16 +10110,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -9662,10 +10129,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -9681,15 +10148,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -9708,16 +10181,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -9726,16 +10200,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -9744,16 +10219,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -9774,7 +10250,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -9782,7 +10258,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -9795,17 +10271,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -9813,10 +10278,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -9837,7 +10302,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -9846,14 +10311,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -9867,7 +10332,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -9883,8 +10348,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -9900,17 +10365,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -9918,8 +10372,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -10532,8 +10992,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>-1</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>596348</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -10564,12 +11024,12 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>185530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>578827</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>602974</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -10605,23 +11065,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>134985</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>66</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBD0458F-259B-4346-8BB1-96813FCA5E6A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EF1E1EB-20C1-4A02-BA9C-BB3D00E7B671}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10993,48 +11453,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41">
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="Q1" s="55" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="Q1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AD1" s="55" t="s">
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
+      <c r="AD1" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
-      <c r="AI1" s="55"/>
-      <c r="AJ1" s="55"/>
-      <c r="AK1" s="55"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="55"/>
-      <c r="AN1" s="55"/>
-      <c r="AO1" s="55"/>
+      <c r="AE1" s="59"/>
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="59"/>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="59"/>
+      <c r="AK1" s="59"/>
+      <c r="AL1" s="59"/>
+      <c r="AM1" s="59"/>
+      <c r="AN1" s="59"/>
+      <c r="AO1" s="59"/>
     </row>
     <row r="2" spans="1:41">
       <c r="A2" s="5" t="s">
@@ -12587,13 +13047,13 @@
       <c r="Y22" s="2"/>
     </row>
     <row r="23" spans="1:25">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="58" t="s">
         <v>146</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
       <c r="R23" s="9" t="s">
         <v>5</v>
       </c>
@@ -12605,13 +13065,13 @@
       <c r="Y23" s="2"/>
     </row>
     <row r="24" spans="1:25">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
       <c r="R24" s="9" t="s">
         <v>7</v>
       </c>
@@ -12623,13 +13083,13 @@
       <c r="Y24" s="2"/>
     </row>
     <row r="25" spans="1:25">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="58" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
       <c r="R25" s="9" t="s">
         <v>6</v>
       </c>
@@ -12815,8 +13275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7456461C-E2A3-44D7-A21C-7E2601ED2580}">
   <dimension ref="A1:AN29"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="T47" sqref="T47"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12826,29 +13286,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
       <c r="J1" s="40"/>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="18" t="s">
@@ -12907,7 +13367,7 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" t="s">
+      <c r="A3" s="56" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="1">
@@ -12934,7 +13394,7 @@
       <c r="I3" s="1">
         <v>0.1054961160521711</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="56" t="s">
         <v>46</v>
       </c>
       <c r="L3" s="3">
@@ -12963,7 +13423,7 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" t="s">
+      <c r="A4" s="56" t="s">
         <v>113</v>
       </c>
       <c r="B4" s="1">
@@ -12990,8 +13450,8 @@
       <c r="I4" s="1">
         <v>7.56835729174863E-2</v>
       </c>
-      <c r="K4" s="18" t="s">
-        <v>57</v>
+      <c r="K4" s="56" t="s">
+        <v>113</v>
       </c>
       <c r="L4" s="3">
         <v>0.15795795000000001</v>
@@ -13019,8 +13479,8 @@
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" t="s">
-        <v>110</v>
+      <c r="A5" s="56" t="s">
+        <v>181</v>
       </c>
       <c r="B5" s="1">
         <v>0.1001653605223721</v>
@@ -13046,8 +13506,8 @@
       <c r="I5" s="1">
         <v>0.11233215045429397</v>
       </c>
-      <c r="K5" s="18" t="s">
-        <v>56</v>
+      <c r="K5" s="56" t="s">
+        <v>181</v>
       </c>
       <c r="L5" s="3">
         <v>0.20241644</v>
@@ -13075,8 +13535,8 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" t="s">
-        <v>111</v>
+      <c r="A6" s="56" t="s">
+        <v>182</v>
       </c>
       <c r="B6" s="1">
         <v>0.42996072770301946</v>
@@ -13102,8 +13562,8 @@
       <c r="I6" s="1">
         <v>0.50104182992018786</v>
       </c>
-      <c r="K6" s="18" t="s">
-        <v>54</v>
+      <c r="K6" s="56" t="s">
+        <v>182</v>
       </c>
       <c r="L6" s="3">
         <v>0.25003483999999998</v>
@@ -13131,8 +13591,8 @@
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" t="s">
-        <v>112</v>
+      <c r="A7" s="56" t="s">
+        <v>183</v>
       </c>
       <c r="B7" s="1">
         <v>0.2213799883507718</v>
@@ -13158,8 +13618,8 @@
       <c r="I7" s="1">
         <v>0.32756816462582083</v>
       </c>
-      <c r="K7" s="18" t="s">
-        <v>55</v>
+      <c r="K7" s="56" t="s">
+        <v>183</v>
       </c>
       <c r="L7" s="3">
         <v>0.35201194000000002</v>
@@ -13187,7 +13647,7 @@
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" t="s">
+      <c r="A8" s="56" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="1">
@@ -13214,7 +13674,7 @@
       <c r="I8" s="1">
         <v>5.0066456251550172E-2</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="56" t="s">
         <v>47</v>
       </c>
       <c r="L8" s="3">
@@ -13243,7 +13703,7 @@
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" t="s">
+      <c r="A9" s="56" t="s">
         <v>48</v>
       </c>
       <c r="B9" s="1">
@@ -13270,7 +13730,7 @@
       <c r="I9" s="3">
         <v>0.50518975920166476</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="56" t="s">
         <v>48</v>
       </c>
       <c r="L9" s="3">
@@ -13299,7 +13759,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" t="s">
+      <c r="A10" s="56" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="1">
@@ -13326,7 +13786,7 @@
       <c r="I10" s="3">
         <v>4.7846889952153108E-3</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="K10" s="56" t="s">
         <v>49</v>
       </c>
       <c r="L10" s="3">
@@ -13355,7 +13815,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" t="s">
+      <c r="A11" s="56" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="1">
@@ -13382,7 +13842,7 @@
       <c r="I11" s="1">
         <v>6.5596874850248704E-2</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="56" t="s">
         <v>50</v>
       </c>
       <c r="L11" s="3">
@@ -13411,7 +13871,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" t="s">
+      <c r="A12" s="56" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="1">
@@ -13438,7 +13898,7 @@
       <c r="I12" s="1">
         <v>2.0165847517132858E-2</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="56" t="s">
         <v>51</v>
       </c>
       <c r="L12" s="3">
@@ -13467,7 +13927,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" t="s">
+      <c r="A13" s="56" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="1">
@@ -13494,7 +13954,7 @@
       <c r="I13" s="1">
         <v>6.1271956632230472E-2</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="56" t="s">
         <v>52</v>
       </c>
       <c r="L13" s="3">
@@ -13523,7 +13983,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" t="s">
+      <c r="A14" s="56" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="1">
@@ -13550,7 +14010,7 @@
       <c r="I14" s="1">
         <v>3.4205709129131311E-2</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="56" t="s">
         <v>53</v>
       </c>
       <c r="L14" s="3">
@@ -13718,8 +14178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB317F8-1811-40BD-9FF4-3B66CC20E864}">
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P57" sqref="P57:P69"/>
+    <sheetView topLeftCell="H31" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35:M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14290,13 +14750,13 @@
       </c>
     </row>
     <row r="13" spans="1:28">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
     </row>
     <row r="14" spans="1:28">
       <c r="A14" s="16" t="s">
@@ -15268,18 +15728,18 @@
       </c>
     </row>
     <row r="33" spans="1:17">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="60" t="s">
         <v>149</v>
       </c>
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
     </row>
     <row r="34" spans="1:17">
       <c r="C34" s="18" t="s">
@@ -15319,7 +15779,7 @@
         <v>154</v>
       </c>
       <c r="Q34" s="4" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -15407,7 +15867,7 @@
         <v>3425.3088677929909</v>
       </c>
       <c r="M36" s="27" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="N36" s="17">
         <v>1286.7185755809573</v>
@@ -15460,7 +15920,7 @@
         <v>1286.7185755809573</v>
       </c>
       <c r="M37" s="27" t="s">
-        <v>56</v>
+        <v>181</v>
       </c>
       <c r="N37" s="17">
         <v>2465.2051662102749</v>
@@ -15513,7 +15973,7 @@
         <v>2465.2051662102749</v>
       </c>
       <c r="M38" s="27" t="s">
-        <v>54</v>
+        <v>182</v>
       </c>
       <c r="N38" s="17">
         <v>4376.6472184650174</v>
@@ -15566,7 +16026,7 @@
         <v>4376.6472184650174</v>
       </c>
       <c r="M39" s="27" t="s">
-        <v>55</v>
+        <v>183</v>
       </c>
       <c r="N39" s="17">
         <v>2235.1033002386639</v>
@@ -16002,59 +16462,59 @@
       </c>
     </row>
     <row r="56" spans="2:16">
-      <c r="B56" s="56" t="s">
-        <v>156</v>
-      </c>
-      <c r="C56" s="56"/>
-      <c r="D56" s="56"/>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="56"/>
-      <c r="H56" s="56"/>
-      <c r="I56" s="56"/>
-      <c r="J56" s="56"/>
-      <c r="K56" s="56"/>
-      <c r="L56" s="56"/>
+      <c r="B56" s="60" t="s">
+        <v>155</v>
+      </c>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="60"/>
+      <c r="F56" s="60"/>
+      <c r="G56" s="60"/>
+      <c r="H56" s="60"/>
+      <c r="I56" s="60"/>
+      <c r="J56" s="60"/>
+      <c r="K56" s="60"/>
+      <c r="L56" s="60"/>
     </row>
     <row r="57" spans="2:16">
       <c r="B57" s="4" t="s">
         <v>109</v>
       </c>
       <c r="C57" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="D57" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="D57" s="42" t="s">
+      <c r="E57" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="E57" s="42" t="s">
+      <c r="F57" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="F57" s="48" t="s">
+      <c r="G57" s="48" t="s">
         <v>161</v>
       </c>
-      <c r="G57" s="48" t="s">
+      <c r="H57" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="H57" s="48" t="s">
+      <c r="I57" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="I57" s="48" t="s">
+      <c r="J57" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="J57" s="48" t="s">
+      <c r="K57" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="K57" s="42" t="s">
-        <v>166</v>
-      </c>
       <c r="L57" s="42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O57" s="4" t="s">
         <v>109</v>
       </c>
       <c r="P57" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="2:16">
@@ -16582,10 +17042,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46015174-E766-4E6A-9E50-9EC594E0B4D4}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16601,42 +17062,42 @@
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="17" max="19" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="L1" s="55" t="s">
-        <v>174</v>
-      </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="L1" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" t="s">
@@ -16667,26 +17128,26 @@
         <v>68</v>
       </c>
       <c r="J2" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K2" s="51"/>
       <c r="L2" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="M2" s="59" t="s">
         <v>175</v>
       </c>
-      <c r="M2" s="55" t="s">
-        <v>176</v>
-      </c>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
       <c r="W2" s="52" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -17268,25 +17729,25 @@
       </c>
       <c r="K14" s="49"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:21">
       <c r="A17" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="C17" s="52" t="s">
         <v>168</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="D17" s="52" t="s">
         <v>169</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="E17" s="52" t="s">
         <v>170</v>
       </c>
-      <c r="E17" s="52" t="s">
-        <v>171</v>
-      </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -17300,10 +17761,38 @@
         <v>2.4883994999999999E-2</v>
       </c>
       <c r="E18" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>171</v>
+      </c>
+      <c r="L18" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="M18" s="55" t="s">
+        <v>157</v>
+      </c>
+      <c r="N18" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="O18" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="P18" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q18" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="R18" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="S18" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="T18" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="U18" s="54"/>
+    </row>
+    <row r="19" spans="1:21" hidden="1">
       <c r="A19" t="s">
         <v>111</v>
       </c>
@@ -17319,8 +17808,36 @@
       <c r="E19" s="53">
         <v>-1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="L19" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0.31619371320508294</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0.16207543018844645</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0.360817657800581</v>
+      </c>
+      <c r="P19" s="1">
+        <v>0.24602546786115667</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0.14562871999866411</v>
+      </c>
+      <c r="R19" s="1">
+        <v>0.30457568239097665</v>
+      </c>
+      <c r="S19" s="1">
+        <v>0.34833551113640071</v>
+      </c>
+      <c r="T19" s="1">
+        <v>0.48762200648671372</v>
+      </c>
+      <c r="U19" s="49"/>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
         <v>111</v>
       </c>
@@ -17334,10 +17851,38 @@
         <v>3.5691899999999999E-2</v>
       </c>
       <c r="E20" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>171</v>
+      </c>
+      <c r="L20" s="55" t="s">
+        <v>178</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.27181547323372851</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0.17861077444078158</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0.29065802642113286</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0.23699432045688906</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0.10887560949091929</v>
+      </c>
+      <c r="R20" s="1">
+        <v>0.2013734495507056</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0.19940061345749924</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0.42220770848218803</v>
+      </c>
+      <c r="U20" s="49"/>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
         <v>111</v>
       </c>
@@ -17351,10 +17896,45 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E21" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>171</v>
+      </c>
+      <c r="L21" s="55" t="s">
+        <v>176</v>
+      </c>
+      <c r="M21" s="1">
+        <f>M19-M20</f>
+        <v>4.4378239971354427E-2</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" ref="N21:T21" si="0">N19-N20</f>
+        <v>-1.6535344252335132E-2</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="0"/>
+        <v>7.015963137944814E-2</v>
+      </c>
+      <c r="P21" s="1">
+        <f t="shared" si="0"/>
+        <v>9.0311474042676088E-3</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6753110507744824E-2</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10320223284027105</v>
+      </c>
+      <c r="S21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.14893489767890147</v>
+      </c>
+      <c r="T21" s="1">
+        <f t="shared" si="0"/>
+        <v>6.5414298004525695E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -17368,10 +17948,37 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E22" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>171</v>
+      </c>
+      <c r="L22" s="55" t="s">
+        <v>180</v>
+      </c>
+      <c r="M22" s="57">
+        <v>3.5</v>
+      </c>
+      <c r="N22" s="57">
+        <v>2</v>
+      </c>
+      <c r="O22" s="57">
+        <v>5.5</v>
+      </c>
+      <c r="P22" s="57">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="57">
+        <v>3.5</v>
+      </c>
+      <c r="R22" s="57">
+        <v>7</v>
+      </c>
+      <c r="S22" s="57">
+        <v>8</v>
+      </c>
+      <c r="T22" s="57">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
         <v>111</v>
       </c>
@@ -17385,10 +17992,10 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E23" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -17402,10 +18009,10 @@
         <v>1.7960477999999998E-2</v>
       </c>
       <c r="E24" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -17419,10 +18026,14 @@
         <v>1.1616045E-2</v>
       </c>
       <c r="E25" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>171</v>
+      </c>
+      <c r="L25" s="55"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -17436,10 +18047,25 @@
         <v>1.1616045E-2</v>
       </c>
       <c r="E26" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>171</v>
+      </c>
+      <c r="L26" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="M26" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="N26" s="55" t="s">
+        <v>178</v>
+      </c>
+      <c r="O26" s="55" t="s">
+        <v>176</v>
+      </c>
+      <c r="P26" s="55" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
         <v>111</v>
       </c>
@@ -17453,10 +18079,25 @@
         <v>1.1616045E-2</v>
       </c>
       <c r="E27" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>171</v>
+      </c>
+      <c r="L27" s="55" t="s">
+        <v>157</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0.31619371320508294</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0.27181547323372851</v>
+      </c>
+      <c r="O27" s="1">
+        <v>4.4378239971354427E-2</v>
+      </c>
+      <c r="P27" s="57">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -17470,10 +18111,25 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E28" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>171</v>
+      </c>
+      <c r="L28" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0.16207543018844645</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0.17861077444078158</v>
+      </c>
+      <c r="O28" s="1">
+        <v>1.6535344252335101E-2</v>
+      </c>
+      <c r="P28" s="57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" hidden="1">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -17489,8 +18145,23 @@
       <c r="E29" s="53">
         <v>-1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="L29" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0.360817657800581</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0.29065802642113286</v>
+      </c>
+      <c r="O29" s="1">
+        <v>7.015963137944814E-2</v>
+      </c>
+      <c r="P29" s="57">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" hidden="1">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -17506,8 +18177,23 @@
       <c r="E30" s="53">
         <v>-1</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="L30" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="M30" s="1">
+        <v>0.24602546786115667</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0.23699432045688906</v>
+      </c>
+      <c r="O30" s="1">
+        <v>9.0311474042676088E-3</v>
+      </c>
+      <c r="P30" s="57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" t="s">
         <v>112</v>
       </c>
@@ -17521,10 +18207,25 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E31" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>171</v>
+      </c>
+      <c r="L31" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="M31" s="1">
+        <v>0.14562871999866411</v>
+      </c>
+      <c r="N31" s="1">
+        <v>0.10887560949091929</v>
+      </c>
+      <c r="O31" s="1">
+        <v>3.6753110507744824E-2</v>
+      </c>
+      <c r="P31" s="57">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -17538,10 +18239,25 @@
         <v>1.7290281000000001E-2</v>
       </c>
       <c r="E32" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>171</v>
+      </c>
+      <c r="L32" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="M32" s="1">
+        <v>0.30457568239097665</v>
+      </c>
+      <c r="N32" s="1">
+        <v>0.2013734495507056</v>
+      </c>
+      <c r="O32" s="1">
+        <v>0.10320223284027105</v>
+      </c>
+      <c r="P32" s="57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -17555,10 +18271,25 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E33" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>171</v>
+      </c>
+      <c r="L33" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0.34833551113640071</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0.19940061345749924</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0.14893489767890147</v>
+      </c>
+      <c r="P33" s="57">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>112</v>
       </c>
@@ -17572,10 +18303,25 @@
         <v>1.1616045E-2</v>
       </c>
       <c r="E34" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>171</v>
+      </c>
+      <c r="L34" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0.48762200648671372</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0.42220770848218803</v>
+      </c>
+      <c r="O34" s="1">
+        <v>6.5414298004525695E-2</v>
+      </c>
+      <c r="P34" s="57">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>112</v>
       </c>
@@ -17589,10 +18335,14 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E35" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>171</v>
+      </c>
+      <c r="P35" s="57">
+        <f>SUM(P27:P34)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>112</v>
       </c>
@@ -17606,10 +18356,10 @@
         <v>1.1616045E-2</v>
       </c>
       <c r="E36" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>112</v>
       </c>
@@ -17623,10 +18373,10 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E37" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -17640,10 +18390,10 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E38" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" hidden="1">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -17660,7 +18410,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -17674,10 +18424,10 @@
         <v>2.0706216E-2</v>
       </c>
       <c r="E40" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" hidden="1">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -17694,7 +18444,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -17708,10 +18458,10 @@
         <v>3.5465864999999999E-2</v>
       </c>
       <c r="E42" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -17725,10 +18475,10 @@
         <v>2.4883994999999999E-2</v>
       </c>
       <c r="E43" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -17742,10 +18492,10 @@
         <v>4.2062732999999998E-2</v>
       </c>
       <c r="E44" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -17759,10 +18509,10 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E45" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -17776,10 +18526,10 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E46" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -17793,10 +18543,10 @@
         <v>1.1616045E-2</v>
       </c>
       <c r="E47" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" hidden="1">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -17827,7 +18577,7 @@
         <v>2.0706216E-2</v>
       </c>
       <c r="E49" s="53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -17844,7 +18594,7 @@
         <v>1.1310671E-2</v>
       </c>
       <c r="E50" s="53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -17861,10 +18611,10 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E51" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" hidden="1">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -17895,7 +18645,7 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E53" s="53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -17912,7 +18662,7 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E54" s="53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -17929,10 +18679,10 @@
         <v>1.1616045E-2</v>
       </c>
       <c r="E55" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" hidden="1">
       <c r="A56" t="s">
         <v>110</v>
       </c>
@@ -17949,7 +18699,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" hidden="1">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -17966,7 +18716,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" hidden="1">
       <c r="A58" t="s">
         <v>110</v>
       </c>
@@ -17983,7 +18733,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" hidden="1">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -18000,7 +18750,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" hidden="1">
       <c r="A60" t="s">
         <v>110</v>
       </c>
@@ -18031,7 +18781,7 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E61" s="53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -18048,10 +18798,10 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E62" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" hidden="1">
       <c r="A63" t="s">
         <v>47</v>
       </c>
@@ -18068,7 +18818,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" hidden="1">
       <c r="A64" t="s">
         <v>47</v>
       </c>
@@ -18085,7 +18835,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" hidden="1">
       <c r="A65" t="s">
         <v>47</v>
       </c>
@@ -18102,7 +18852,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" hidden="1">
       <c r="A66" t="s">
         <v>47</v>
       </c>
@@ -18133,7 +18883,7 @@
         <v>1.7290281000000001E-2</v>
       </c>
       <c r="E67" s="53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -18150,10 +18900,10 @@
         <v>1.1616045E-2</v>
       </c>
       <c r="E68" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" hidden="1">
       <c r="A69" t="s">
         <v>50</v>
       </c>
@@ -18170,7 +18920,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" hidden="1">
       <c r="A70" t="s">
         <v>50</v>
       </c>
@@ -18187,7 +18937,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" hidden="1">
       <c r="A71" t="s">
         <v>50</v>
       </c>
@@ -18218,7 +18968,7 @@
         <v>2.7991815E-2</v>
       </c>
       <c r="E72" s="53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -18235,10 +18985,10 @@
         <v>1.1310671E-2</v>
       </c>
       <c r="E73" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" hidden="1">
       <c r="A74" t="s">
         <v>53</v>
       </c>
@@ -18255,7 +19005,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" hidden="1">
       <c r="A75" t="s">
         <v>53</v>
       </c>
@@ -18272,7 +19022,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" hidden="1">
       <c r="A76" t="s">
         <v>53</v>
       </c>
@@ -18303,10 +19053,10 @@
         <v>1.1616045E-2</v>
       </c>
       <c r="E77" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" hidden="1">
       <c r="A78" t="s">
         <v>51</v>
       </c>
@@ -18323,7 +19073,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" hidden="1">
       <c r="A79" t="s">
         <v>51</v>
       </c>
@@ -18354,7 +19104,7 @@
         <v>1.7755923E-2</v>
       </c>
       <c r="E80" s="53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -18371,7 +19121,7 @@
         <v>1.7290281000000001E-2</v>
       </c>
       <c r="E81" s="53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -18388,10 +19138,10 @@
         <v>1.1718686000000001E-2</v>
       </c>
       <c r="E82" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" hidden="1">
       <c r="A83" t="s">
         <v>113</v>
       </c>
@@ -18409,15 +19159,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E17:E83" xr:uid="{BEA61A31-5D14-414B-87C5-0D47B1111BA9}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J14">
-    <sortCondition ref="J2"/>
+  <autoFilter ref="E17:E83" xr:uid="{BEA61A31-5D14-414B-87C5-0D47B1111BA9}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="s"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L27:P34">
+    <sortCondition ref="L26"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="M2:V2"/>
     <mergeCell ref="L1:W1"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>